<commit_message>
Look up hopper voltage for solution range
</commit_message>
<xml_diff>
--- a/steamworks/conf/shooter_data.xlsx
+++ b/steamworks/conf/shooter_data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/sf/steamworks/conf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/sfng/robots-cpp/steamworks/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:F170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -438,7 +438,7 @@
       <c r="D2" s="4">
         <v>440.27514384998631</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <v>8</v>
       </c>
       <c r="F2" s="6">
@@ -458,8 +458,8 @@
       <c r="D3" s="4">
         <v>440.62782300435993</v>
       </c>
-      <c r="E3" s="3">
-        <v>8</v>
+      <c r="E3" s="6">
+        <v>8.0476190476190474</v>
       </c>
       <c r="F3" s="6">
         <v>0.35267915437361808</v>
@@ -478,8 +478,8 @@
       <c r="D4" s="4">
         <v>441.02827356885882</v>
       </c>
-      <c r="E4" s="3">
-        <v>8</v>
+      <c r="E4" s="6">
+        <v>8.0952380952380949</v>
       </c>
       <c r="F4" s="6">
         <v>0.40045056449889671</v>
@@ -498,8 +498,8 @@
       <c r="D5" s="4">
         <v>441.48299817210409</v>
       </c>
-      <c r="E5" s="3">
-        <v>8</v>
+      <c r="E5" s="6">
+        <v>8.1428571428571423</v>
       </c>
       <c r="F5" s="6">
         <v>0.45472460324526764</v>
@@ -518,8 +518,8 @@
       <c r="D6" s="4">
         <v>441.99711144930097</v>
       </c>
-      <c r="E6" s="3">
-        <v>8</v>
+      <c r="E6" s="6">
+        <v>8.1904761904761898</v>
       </c>
       <c r="F6" s="6">
         <v>0.51411327719688416</v>
@@ -538,8 +538,8 @@
       <c r="D7" s="4">
         <v>442.57445352221384</v>
       </c>
-      <c r="E7" s="3">
-        <v>8</v>
+      <c r="E7" s="6">
+        <v>8.2380952380952372</v>
       </c>
       <c r="F7" s="6">
         <v>0.57734207291287021</v>
@@ -558,8 +558,8 @@
       <c r="D8" s="4">
         <v>443.21769866434897</v>
       </c>
-      <c r="E8" s="3">
-        <v>8</v>
+      <c r="E8" s="6">
+        <v>8.2857142857142847</v>
       </c>
       <c r="F8" s="6">
         <v>0.64324514213512884</v>
@@ -578,8 +578,8 @@
       <c r="D9" s="4">
         <v>443.92845923987898</v>
       </c>
-      <c r="E9" s="3">
-        <v>8</v>
+      <c r="E9" s="6">
+        <v>8.3333333333333321</v>
       </c>
       <c r="F9" s="6">
         <v>0.71076057553000282</v>
@@ -598,8 +598,8 @@
       <c r="D10" s="4">
         <v>444.70738500496645</v>
       </c>
-      <c r="E10" s="3">
-        <v>8</v>
+      <c r="E10" s="6">
+        <v>8.3809523809523796</v>
       </c>
       <c r="F10" s="6">
         <v>0.77892576508747879</v>
@@ -618,8 +618,8 @@
       <c r="D11" s="4">
         <v>445.55425785993339</v>
       </c>
-      <c r="E11" s="3">
-        <v>8</v>
+      <c r="E11" s="6">
+        <v>8.428571428571427</v>
       </c>
       <c r="F11" s="6">
         <v>0.84687285496693221</v>
@@ -638,8 +638,8 @@
       <c r="D12" s="4">
         <v>446.46808214099929</v>
       </c>
-      <c r="E12" s="3">
-        <v>8</v>
+      <c r="E12" s="6">
+        <v>8.4761904761904745</v>
       </c>
       <c r="F12" s="6">
         <v>0.91382428106589941</v>
@@ -658,8 +658,8 @@
       <c r="D13" s="4">
         <v>447.44717054000557</v>
       </c>
-      <c r="E13" s="3">
-        <v>8</v>
+      <c r="E13" s="6">
+        <v>8.5238095238095219</v>
       </c>
       <c r="F13" s="6">
         <v>0.97908839900628664</v>
@@ -678,8 +678,8 @@
       <c r="D14" s="4">
         <v>448.48922574087464</v>
       </c>
-      <c r="E14" s="3">
-        <v>8</v>
+      <c r="E14" s="6">
+        <v>8.5714285714285694</v>
       </c>
       <c r="F14" s="6">
         <v>1.042055200869072</v>
@@ -698,8 +698,8 @@
       <c r="D15" s="4">
         <v>449.59141786130476</v>
       </c>
-      <c r="E15" s="3">
-        <v>8</v>
+      <c r="E15" s="6">
+        <v>8.6190476190476168</v>
       </c>
       <c r="F15" s="6">
         <v>1.1021921204301179</v>
@@ -718,8 +718,8 @@
       <c r="D16" s="4">
         <v>450.75045778817275</v>
       </c>
-      <c r="E16" s="3">
-        <v>8</v>
+      <c r="E16" s="6">
+        <v>8.6666666666666643</v>
       </c>
       <c r="F16" s="6">
         <v>1.1590399268679903</v>
@@ -738,8 +738,8 @@
       <c r="D17" s="4">
         <v>451.96266649545123</v>
       </c>
-      <c r="E17" s="3">
-        <v>8</v>
+      <c r="E17" s="6">
+        <v>8.7142857142857117</v>
       </c>
       <c r="F17" s="6">
         <v>1.212208707278478</v>
@@ -758,8 +758,8 @@
       <c r="D18" s="4">
         <v>453.22404043302868</v>
       </c>
-      <c r="E18" s="3">
-        <v>8</v>
+      <c r="E18" s="6">
+        <v>8.7619047619047592</v>
       </c>
       <c r="F18" s="6">
         <v>1.2613739375774458</v>
@@ -778,8 +778,8 @@
       <c r="D19" s="4">
         <v>454.53031307500987</v>
       </c>
-      <c r="E19" s="3">
-        <v>8</v>
+      <c r="E19" s="6">
+        <v>8.8095238095238066</v>
       </c>
       <c r="F19" s="6">
         <v>1.3062726419811952</v>
@@ -798,8 +798,8 @@
       <c r="D20" s="4">
         <v>455.8770127163798</v>
       </c>
-      <c r="E20" s="3">
-        <v>8</v>
+      <c r="E20" s="6">
+        <v>8.8571428571428541</v>
       </c>
       <c r="F20" s="6">
         <v>1.3466996413699235</v>
@@ -818,8 +818,8 @@
       <c r="D21" s="4">
         <v>457.25951660599367</v>
       </c>
-      <c r="E21" s="3">
-        <v>8</v>
+      <c r="E21" s="6">
+        <v>8.9047619047619015</v>
       </c>
       <c r="F21" s="6">
         <v>1.3825038896138722</v>
@@ -838,8 +838,8 @@
       <c r="D22" s="4">
         <v>458.67310150524554</v>
       </c>
-      <c r="E22" s="3">
-        <v>8</v>
+      <c r="E22" s="6">
+        <v>8.952380952380949</v>
       </c>
       <c r="F22" s="6">
         <v>1.4135848992518731</v>
@@ -858,8 +858,8 @@
       <c r="D23" s="4">
         <v>460.11299076028354</v>
       </c>
-      <c r="E23" s="3">
-        <v>8</v>
+      <c r="E23" s="6">
+        <v>8.9999999999999964</v>
       </c>
       <c r="F23" s="6">
         <v>1.4398892550379969</v>
@@ -878,8 +878,8 @@
       <c r="D24" s="4">
         <v>461.57439797681855</v>
       </c>
-      <c r="E24" s="3">
-        <v>8</v>
+      <c r="E24" s="6">
+        <v>9.0476190476190439</v>
       </c>
       <c r="F24" s="6">
         <v>1.461407216535008</v>
@@ -898,8 +898,8 @@
       <c r="D25" s="4">
         <v>463.05256738591834</v>
       </c>
-      <c r="E25" s="3">
-        <v>8</v>
+      <c r="E25" s="6">
+        <v>9.0952380952380913</v>
       </c>
       <c r="F25" s="6">
         <v>1.4781694090997917</v>
@@ -918,8 +918,8 @@
       <c r="D26" s="4">
         <v>464.54281098940828</v>
       </c>
-      <c r="E26" s="3">
-        <v>8</v>
+      <c r="E26" s="6">
+        <v>9.1428571428571388</v>
       </c>
       <c r="F26" s="6">
         <v>1.4902436034899438</v>
@@ -938,8 +938,8 @@
       <c r="D27" s="4">
         <v>466.04054257343068</v>
       </c>
-      <c r="E27" s="3">
-        <v>8</v>
+      <c r="E27" s="6">
+        <v>9.1904761904761862</v>
       </c>
       <c r="F27" s="6">
         <v>1.4977315840224037</v>
@@ -958,8 +958,8 @@
       <c r="D28" s="4">
         <v>467.54130867869662</v>
       </c>
-      <c r="E28" s="3">
-        <v>8</v>
+      <c r="E28" s="6">
+        <v>9.2380952380952337</v>
       </c>
       <c r="F28" s="6">
         <v>1.5007661052659387</v>
@@ -978,8 +978,8 @@
       <c r="D29" s="4">
         <v>469.04081661616055</v>
       </c>
-      <c r="E29" s="3">
-        <v>8</v>
+      <c r="E29" s="6">
+        <v>9.2857142857142811</v>
       </c>
       <c r="F29" s="6">
         <v>1.4995079374639317</v>
@@ -998,8 +998,8 @@
       <c r="D30" s="4">
         <v>470.53495961657154</v>
       </c>
-      <c r="E30" s="3">
-        <v>8</v>
+      <c r="E30" s="6">
+        <v>9.3333333333333286</v>
       </c>
       <c r="F30" s="6">
         <v>1.4941430004109861</v>
@@ -1018,8 +1018,8 @@
       <c r="D31" s="4">
         <v>472.01983920236944</v>
       </c>
-      <c r="E31" s="3">
-        <v>8</v>
+      <c r="E31" s="6">
+        <v>9.380952380952376</v>
       </c>
       <c r="F31" s="6">
         <v>1.4848795857978985</v>
@@ -1038,8 +1038,8 @@
       <c r="D32" s="4">
         <v>473.49178487111476</v>
       </c>
-      <c r="E32" s="3">
-        <v>8</v>
+      <c r="E32" s="6">
+        <v>9.4285714285714235</v>
       </c>
       <c r="F32" s="6">
         <v>1.4719456687453203</v>
@@ -1058,8 +1058,8 @@
       <c r="D33" s="4">
         <v>474.94737117773457</v>
       </c>
-      <c r="E33" s="3">
-        <v>8</v>
+      <c r="E33" s="6">
+        <v>9.4761904761904709</v>
       </c>
       <c r="F33" s="6">
         <v>1.4555863066198071</v>
@@ -1078,8 +1078,8 @@
       <c r="D34" s="4">
         <v>476.38343230588634</v>
       </c>
-      <c r="E34" s="3">
-        <v>8</v>
+      <c r="E34" s="6">
+        <v>9.5238095238095184</v>
       </c>
       <c r="F34" s="6">
         <v>1.4360611281517777</v>
@@ -1098,8 +1098,8 @@
       <c r="D35" s="4">
         <v>477.79707421544572</v>
       </c>
-      <c r="E35" s="3">
-        <v>8</v>
+      <c r="E35" s="6">
+        <v>9.5714285714285658</v>
       </c>
       <c r="F35" s="6">
         <v>1.4136419095593737</v>
@@ -1118,8 +1118,8 @@
       <c r="D36" s="4">
         <v>479.18568445575056</v>
       </c>
-      <c r="E36" s="3">
-        <v>8</v>
+      <c r="E36" s="6">
+        <v>9.6190476190476133</v>
       </c>
       <c r="F36" s="6">
         <v>1.3886102403048426</v>
@@ -1138,8 +1138,8 @@
       <c r="D37" s="4">
         <v>480.54693973269877</v>
       </c>
-      <c r="E37" s="3">
-        <v>8</v>
+      <c r="E37" s="6">
+        <v>9.6666666666666607</v>
       </c>
       <c r="F37" s="6">
         <v>1.3612552769482136</v>
@@ -1158,8 +1158,8 @@
       <c r="D38" s="4">
         <v>481.87881131825543</v>
       </c>
-      <c r="E38" s="3">
-        <v>8</v>
+      <c r="E38" s="6">
+        <v>9.7142857142857082</v>
       </c>
       <c r="F38" s="6">
         <v>1.3318715855566552</v>
@@ -1178,8 +1178,8 @@
       <c r="D39" s="4">
         <v>483.17956839119415</v>
       </c>
-      <c r="E39" s="3">
-        <v>8</v>
+      <c r="E39" s="6">
+        <v>9.7619047619047556</v>
       </c>
       <c r="F39" s="6">
         <v>1.3007570729387226</v>
@@ -1198,8 +1198,8 @@
       <c r="D40" s="4">
         <v>484.44777939768665</v>
       </c>
-      <c r="E40" s="3">
-        <v>8</v>
+      <c r="E40" s="6">
+        <v>9.8095238095238031</v>
       </c>
       <c r="F40" s="6">
         <v>1.2682110064924927</v>
@@ -1218,8 +1218,8 @@
       <c r="D41" s="4">
         <v>485.68231151964119</v>
       </c>
-      <c r="E41" s="3">
-        <v>8</v>
+      <c r="E41" s="6">
+        <v>9.8571428571428505</v>
       </c>
       <c r="F41" s="6">
         <v>1.234532121954544</v>
@@ -1238,8 +1238,8 @@
       <c r="D42" s="4">
         <v>486.8823283406191</v>
       </c>
-      <c r="E42" s="3">
-        <v>8</v>
+      <c r="E42" s="6">
+        <v>9.904761904761898</v>
       </c>
       <c r="F42" s="6">
         <v>1.2000168209779076</v>
@@ -1258,8 +1258,8 @@
       <c r="D43" s="4">
         <v>488.04728579644416</v>
       </c>
-      <c r="E43" s="3">
-        <v>8</v>
+      <c r="E43" s="6">
+        <v>9.9523809523809454</v>
       </c>
       <c r="F43" s="6">
         <v>1.1649574558250606</v>
@@ -1278,8 +1278,8 @@
       <c r="D44" s="4">
         <v>489.17692650033405</v>
       </c>
-      <c r="E44" s="3">
-        <v>8</v>
+      <c r="E44" s="6">
+        <v>9.9999999999999929</v>
       </c>
       <c r="F44" s="6">
         <v>1.1296407038898906</v>
@@ -1298,8 +1298,8 @@
       <c r="D45" s="4">
         <v>490.27127253045455</v>
       </c>
-      <c r="E45" s="3">
-        <v>8</v>
+      <c r="E45" s="6">
+        <v>10.04761904761904</v>
       </c>
       <c r="F45" s="6">
         <v>1.094346030120505</v>
@@ -1318,8 +1318,8 @@
       <c r="D46" s="4">
         <v>491.33061676848865</v>
       </c>
-      <c r="E46" s="3">
-        <v>8</v>
+      <c r="E46" s="6">
+        <v>10.095238095238088</v>
       </c>
       <c r="F46" s="6">
         <v>1.0593442380341003</v>
@@ -1338,8 +1338,8 @@
       <c r="D47" s="4">
         <v>492.35551287815451</v>
       </c>
-      <c r="E47" s="3">
-        <v>8</v>
+      <c r="E47" s="6">
+        <v>10.142857142857135</v>
       </c>
       <c r="F47" s="6">
         <v>1.0248961096658604</v>
@@ -1358,8 +1358,8 @@
       <c r="D48" s="4">
         <v>493.34676401189336</v>
       </c>
-      <c r="E48" s="3">
-        <v>8</v>
+      <c r="E48" s="6">
+        <v>10.190476190476183</v>
       </c>
       <c r="F48" s="6">
         <v>0.99125113373884233</v>
@@ -1378,8 +1378,8 @@
       <c r="D49" s="4">
         <v>494.30541033462487</v>
       </c>
-      <c r="E49" s="3">
-        <v>8</v>
+      <c r="E49" s="6">
+        <v>10.23809523809523</v>
       </c>
       <c r="F49" s="6">
         <v>0.95864632273151074</v>
@@ -1398,8 +1398,8 @@
       <c r="D50" s="4">
         <v>495.23271545273292</v>
       </c>
-      <c r="E50" s="3">
-        <v>8</v>
+      <c r="E50" s="6">
+        <v>10.285714285714278</v>
       </c>
       <c r="F50" s="6">
         <v>0.92730511810805183</v>
@@ -1418,8 +1418,8 @@
       <c r="D51" s="4">
         <v>496.13015183715015</v>
       </c>
-      <c r="E51" s="3">
-        <v>8</v>
+      <c r="E51" s="6">
+        <v>10.333333333333325</v>
       </c>
       <c r="F51" s="6">
         <v>0.89743638441723306</v>
@@ -1438,8 +1438,8 @@
       <c r="D52" s="4">
         <v>496.99938532943179</v>
       </c>
-      <c r="E52" s="3">
-        <v>8</v>
+      <c r="E52" s="6">
+        <v>10.380952380952372</v>
       </c>
       <c r="F52" s="6">
         <v>0.86923349228163715</v>
@@ -1458,8 +1458,8 @@
       <c r="D53" s="4">
         <v>497.84225881863949</v>
       </c>
-      <c r="E53" s="3">
-        <v>8</v>
+      <c r="E53" s="6">
+        <v>10.42857142857142</v>
       </c>
       <c r="F53" s="6">
         <v>0.84287348920770455</v>
@@ -1478,8 +1478,8 @@
       <c r="D54" s="4">
         <v>498.66077517767826</v>
       </c>
-      <c r="E54" s="3">
-        <v>8</v>
+      <c r="E54" s="6">
+        <v>10.476190476190467</v>
       </c>
       <c r="F54" s="6">
         <v>0.8185163590387674</v>
@@ -1498,8 +1498,8 @@
       <c r="D55" s="4">
         <v>499.45707954938825</v>
       </c>
-      <c r="E55" s="3">
-        <v>8</v>
+      <c r="E55" s="6">
+        <v>10.523809523809515</v>
       </c>
       <c r="F55" s="6">
         <v>0.79630437170999357</v>
@@ -1518,8 +1518,8 @@
       <c r="D56" s="4">
         <v>500.23344106768036</v>
       </c>
-      <c r="E56" s="3">
-        <v>8</v>
+      <c r="E56" s="6">
+        <v>10.571428571428562</v>
       </c>
       <c r="F56" s="6">
         <v>0.77636151829210576</v>
@@ -1538,8 +1538,8 @@
       <c r="D57" s="4">
         <v>500.99223410566174</v>
       </c>
-      <c r="E57" s="3">
-        <v>8</v>
+      <c r="E57" s="6">
+        <v>10.61904761904761</v>
       </c>
       <c r="F57" s="6">
         <v>0.75879303798137698</v>
@@ -1558,8 +1558,8 @@
       <c r="D58" s="4">
         <v>501.73591913733526</v>
       </c>
-      <c r="E58" s="3">
-        <v>8</v>
+      <c r="E58" s="6">
+        <v>10.666666666666657</v>
       </c>
       <c r="F58" s="6">
         <v>0.74368503167352173</v>
@@ -1578,8 +1578,8 @@
       <c r="D59" s="4">
         <v>502.46702330170501</v>
       </c>
-      <c r="E59" s="3">
-        <v>8</v>
+      <c r="E59" s="6">
+        <v>10.714285714285705</v>
       </c>
       <c r="F59" s="6">
         <v>0.73110416436975356</v>
@@ -1598,8 +1598,8 @@
       <c r="D60" s="4">
         <v>503.18812075873848</v>
       </c>
-      <c r="E60" s="3">
-        <v>8</v>
+      <c r="E60" s="6">
+        <v>10.761904761904752</v>
       </c>
       <c r="F60" s="6">
         <v>0.72109745703346562</v>
@@ -1618,8 +1618,8 @@
       <c r="D61" s="4">
         <v>503.90181292460602</v>
       </c>
-      <c r="E61" s="3">
-        <v>8</v>
+      <c r="E61" s="6">
+        <v>10.8095238095238</v>
       </c>
       <c r="F61" s="6">
         <v>0.71369216586754192</v>
@@ -1638,8 +1638,8 @@
       <c r="D62" s="4">
         <v>504.61070867562648</v>
       </c>
-      <c r="E62" s="3">
-        <v>8</v>
+      <c r="E62" s="6">
+        <v>10.857142857142847</v>
       </c>
       <c r="F62" s="6">
         <v>0.70889575102046365</v>
@@ -1658,8 +1658,8 @@
       <c r="D63" s="4">
         <v>505.31740460920537</v>
       </c>
-      <c r="E63" s="3">
-        <v>8</v>
+      <c r="E63" s="6">
+        <v>10.904761904761894</v>
       </c>
       <c r="F63" s="6">
         <v>0.70669593357888516</v>
@@ -1678,8 +1678,8 @@
       <c r="D64" s="4">
         <v>506.02446545036491</v>
       </c>
-      <c r="E64" s="3">
-        <v>8</v>
+      <c r="E64" s="6">
+        <v>10.952380952380942</v>
       </c>
       <c r="F64" s="6">
         <v>0.70706084115954582</v>
@@ -1698,8 +1698,8 @@
       <c r="D65" s="4">
         <v>506.7344046920216</v>
       </c>
-      <c r="E65" s="3">
-        <v>8</v>
+      <c r="E65" s="6">
+        <v>10.999999999999989</v>
       </c>
       <c r="F65" s="6">
         <v>0.70993924165668432</v>
@@ -1718,8 +1718,8 @@
       <c r="D66" s="4">
         <v>507.4496655584835</v>
       </c>
-      <c r="E66" s="3">
-        <v>8</v>
+      <c r="E66" s="6">
+        <v>11.047619047619037</v>
       </c>
       <c r="F66" s="6">
         <v>0.71526086646190379</v>
@@ -1738,8 +1738,8 @@
       <c r="D67" s="4">
         <v>508.17260238022118</v>
       </c>
-      <c r="E67" s="3">
-        <v>8</v>
+      <c r="E67" s="6">
+        <v>11.095238095238084</v>
       </c>
       <c r="F67" s="6">
         <v>0.72293682173767593</v>
@@ -1758,8 +1758,8 @@
       <c r="D68" s="4">
         <v>508.90546246811846</v>
       </c>
-      <c r="E68" s="3">
-        <v>8</v>
+      <c r="E68" s="6">
+        <v>11.142857142857132</v>
       </c>
       <c r="F68" s="6">
         <v>0.7328600878972793</v>
@@ -1778,8 +1778,8 @@
       <c r="D69" s="4">
         <v>509.6503685766902</v>
       </c>
-      <c r="E69" s="3">
-        <v>8</v>
+      <c r="E69" s="6">
+        <v>11.190476190476179</v>
       </c>
       <c r="F69" s="6">
         <v>0.74490610857174033</v>
@@ -1798,8 +1798,8 @@
       <c r="D70" s="4">
         <v>510.40930204362212</v>
       </c>
-      <c r="E70" s="3">
-        <v>8</v>
+      <c r="E70" s="6">
+        <v>11.238095238095227</v>
       </c>
       <c r="F70" s="6">
         <v>0.75893346693192143</v>
@@ -1818,8 +1818,8 @@
       <c r="D71" s="4">
         <v>511.18408669597829</v>
       </c>
-      <c r="E71" s="3">
-        <v>8</v>
+      <c r="E71" s="6">
+        <v>11.285714285714274</v>
       </c>
       <c r="F71" s="6">
         <v>0.77478465235617477</v>
@@ -1838,8 +1838,8 @@
       <c r="D72" s="4">
         <v>511.97637360948556</v>
       </c>
-      <c r="E72" s="3">
-        <v>8</v>
+      <c r="E72" s="6">
+        <v>11.333333333333321</v>
       </c>
       <c r="F72" s="6">
         <v>0.79228691350726876</v>
@@ -1858,8 +1858,8 @@
       <c r="D73" s="4">
         <v>512.787626811677</v>
       </c>
-      <c r="E73" s="3">
-        <v>8</v>
+      <c r="E73" s="6">
+        <v>11.380952380952369</v>
       </c>
       <c r="F73" s="6">
         <v>0.81125320219143759</v>
@@ -1878,8 +1878,8 @@
       <c r="D74" s="4">
         <v>513.61911001505632</v>
       </c>
-      <c r="E74" s="3">
-        <v>8</v>
+      <c r="E74" s="6">
+        <v>11.428571428571416</v>
       </c>
       <c r="F74" s="6">
         <v>0.83148320337932091</v>
@@ -1898,8 +1898,8 @@
       <c r="D75" s="4">
         <v>514.47187447174929</v>
       </c>
-      <c r="E75" s="3">
-        <v>8</v>
+      <c r="E75" s="6">
+        <v>11.476190476190464</v>
       </c>
       <c r="F75" s="6">
         <v>0.85276445669296663</v>
@@ -1918,8 +1918,8 @@
       <c r="D76" s="4">
         <v>515.34674803546204</v>
       </c>
-      <c r="E76" s="3">
-        <v>8</v>
+      <c r="E76" s="6">
+        <v>11.523809523809511</v>
       </c>
       <c r="F76" s="6">
         <v>0.87487356371275382</v>
@@ -1938,8 +1938,8 @@
       <c r="D77" s="4">
         <v>516.24432552080816</v>
       </c>
-      <c r="E77" s="3">
-        <v>8</v>
+      <c r="E77" s="6">
+        <v>11.571428571428559</v>
       </c>
       <c r="F77" s="6">
         <v>0.89757748534611892</v>
@@ -1958,8 +1958,8 @@
       <c r="D78" s="4">
         <v>517.16496044892392</v>
       </c>
-      <c r="E78" s="3">
-        <v>8</v>
+      <c r="E78" s="6">
+        <v>11.619047619047606</v>
       </c>
       <c r="F78" s="6">
         <v>0.92063492811575998</v>
@@ -1978,8 +1978,8 @@
       <c r="D79" s="4">
         <v>518.1087582662467</v>
       </c>
-      <c r="E79" s="3">
-        <v>8</v>
+      <c r="E79" s="6">
+        <v>11.666666666666654</v>
       </c>
       <c r="F79" s="6">
         <v>0.94379781732277479</v>
@@ -1998,8 +1998,8 @@
       <c r="D80" s="4">
         <v>519.0755711271222</v>
       </c>
-      <c r="E80" s="3">
-        <v>8</v>
+      <c r="E80" s="6">
+        <v>11.714285714285701</v>
       </c>
       <c r="F80" s="6">
         <v>0.96681286087550689</v>
@@ -2018,8 +2018,8 @@
       <c r="D81" s="4">
         <v>520.0649943272756</v>
       </c>
-      <c r="E81" s="3">
-        <v>8</v>
+      <c r="E81" s="6">
+        <v>11.761904761904749</v>
       </c>
       <c r="F81" s="6">
         <v>0.98942320015339646</v>
@@ -2038,8 +2038,8 @@
       <c r="D82" s="4">
         <v>521.07636447725508</v>
       </c>
-      <c r="E82" s="3">
-        <v>8</v>
+      <c r="E82" s="6">
+        <v>11.809523809523796</v>
       </c>
       <c r="F82" s="6">
         <v>1.0113701499794843</v>
@@ -2058,8 +2058,8 @@
       <c r="D83" s="4">
         <v>522.10875950481113</v>
       </c>
-      <c r="E83" s="3">
-        <v>8</v>
+      <c r="E83" s="6">
+        <v>11.857142857142843</v>
       </c>
       <c r="F83" s="6">
         <v>1.0323950275560492</v>
@@ -2078,8 +2078,8 @@
       <c r="D84" s="4">
         <v>523.16100057359563</v>
       </c>
-      <c r="E84" s="3">
-        <v>8</v>
+      <c r="E84" s="6">
+        <v>11.904761904761891</v>
       </c>
       <c r="F84" s="6">
         <v>1.0522410687844967</v>
@@ -2098,8 +2098,8 @@
       <c r="D85" s="4">
         <v>524.23165600931225</v>
       </c>
-      <c r="E85" s="3">
-        <v>8</v>
+      <c r="E85" s="6">
+        <v>11.952380952380938</v>
       </c>
       <c r="F85" s="6">
         <v>1.0706554357166169</v>
@@ -2118,8 +2118,8 @@
       <c r="D86" s="4">
         <v>525.31904731693339</v>
       </c>
-      <c r="E86" s="3">
-        <v>8</v>
+      <c r="E86" s="6">
+        <v>12</v>
       </c>
       <c r="F86" s="6">
         <v>1.0873913076211466</v>
@@ -2138,8 +2138,8 @@
       <c r="D87" s="4">
         <v>526.42125738526647</v>
       </c>
-      <c r="E87" s="3">
-        <v>8</v>
+      <c r="E87" s="6">
+        <v>12</v>
       </c>
       <c r="F87" s="6">
         <v>1.1022100683330791</v>
@@ -2158,8 +2158,8 @@
       <c r="D88" s="4">
         <v>527.53614095857029</v>
       </c>
-      <c r="E88" s="3">
-        <v>8</v>
+      <c r="E88" s="6">
+        <v>12</v>
       </c>
       <c r="F88" s="6">
         <v>1.114883573303814</v>
@@ -2178,8 +2178,8 @@
       <c r="D89" s="4">
         <v>528.66133747119875</v>
       </c>
-      <c r="E89" s="3">
-        <v>8</v>
+      <c r="E89" s="6">
+        <v>12</v>
       </c>
       <c r="F89" s="6">
         <v>1.1251965126284631</v>
@@ -2198,8 +2198,8 @@
       <c r="D90" s="4">
         <v>529.79428632938198</v>
       </c>
-      <c r="E90" s="3">
-        <v>8</v>
+      <c r="E90" s="6">
+        <v>12</v>
       </c>
       <c r="F90" s="6">
         <v>1.1329488581832265</v>
@@ -2218,8 +2218,8 @@
       <c r="D91" s="4">
         <v>530.93224473091232</v>
       </c>
-      <c r="E91" s="3">
-        <v>8</v>
+      <c r="E91" s="6">
+        <v>12</v>
       </c>
       <c r="F91" s="6">
         <v>1.1379584015303408</v>
@@ -2238,8 +2238,8 @@
       <c r="D92" s="4">
         <v>532.07230810979945</v>
       </c>
-      <c r="E92" s="3">
-        <v>8</v>
+      <c r="E92" s="6">
+        <v>12</v>
       </c>
       <c r="F92" s="6">
         <v>1.1400633788871346</v>
@@ -2258,8 +2258,8 @@
       <c r="D93" s="4">
         <v>533.21143329629831</v>
       </c>
-      <c r="E93" s="3">
-        <v>8</v>
+      <c r="E93" s="6">
+        <v>12</v>
       </c>
       <c r="F93" s="6">
         <v>1.139125186498859</v>
@@ -2278,8 +2278,8 @@
       <c r="D94" s="4">
         <v>534.34646447895193</v>
       </c>
-      <c r="E94" s="3">
-        <v>8</v>
+      <c r="E94" s="6">
+        <v>12</v>
       </c>
       <c r="F94" s="6">
         <v>1.1350311826536199</v>
@@ -2298,8 +2298,8 @@
       <c r="D95" s="4">
         <v>535.47416205867466</v>
       </c>
-      <c r="E95" s="3">
-        <v>8</v>
+      <c r="E95" s="6">
+        <v>12</v>
       </c>
       <c r="F95" s="6">
         <v>1.1276975797227351</v>
@@ -2318,8 +2318,8 @@
       <c r="D96" s="4">
         <v>536.59123448258015</v>
       </c>
-      <c r="E96" s="3">
-        <v>8</v>
+      <c r="E96" s="6">
+        <v>12</v>
       </c>
       <c r="F96" s="6">
         <v>1.1170724239054834</v>
@@ -2338,8 +2338,8 @@
       <c r="D97" s="4">
         <v>537.69437314648803</v>
       </c>
-      <c r="E97" s="3">
-        <v>8</v>
+      <c r="E97" s="6">
+        <v>12</v>
       </c>
       <c r="F97" s="6">
         <v>1.1031386639078846</v>
@@ -2358,8 +2358,8 @@
       <c r="D98" s="4">
         <v>538.780290455451</v>
       </c>
-      <c r="E98" s="3">
-        <v>8</v>
+      <c r="E98" s="6">
+        <v>12</v>
       </c>
       <c r="F98" s="6">
         <v>1.0859173089629621</v>
@@ -2378,8 +2378,8 @@
       <c r="D99" s="4">
         <v>539.8457611285221</v>
       </c>
-      <c r="E99" s="3">
-        <v>8</v>
+      <c r="E99" s="6">
+        <v>12</v>
       </c>
       <c r="F99" s="6">
         <v>1.0654706730711041</v>
@@ -2398,8 +2398,8 @@
       <c r="D100" s="4">
         <v>540.88766683915583</v>
       </c>
-      <c r="E100" s="3">
-        <v>8</v>
+      <c r="E100" s="6">
+        <v>12</v>
       </c>
       <c r="F100" s="6">
         <v>1.0419057106337277</v>
@@ -2418,8 +2418,8 @@
       <c r="D101" s="4">
         <v>541.90304427858337</v>
       </c>
-      <c r="E101" s="3">
-        <v>8</v>
+      <c r="E101" s="6">
+        <v>12</v>
       </c>
       <c r="F101" s="6">
         <v>1.0153774394275388</v>
@@ -2438,8 +2438,8 @@
       <c r="D102" s="4">
         <v>542.8891367293063</v>
       </c>
-      <c r="E102" s="3">
-        <v>8</v>
+      <c r="E102" s="6">
+        <v>12</v>
       </c>
       <c r="F102" s="6">
         <v>0.98609245072293561</v>
@@ -2458,8 +2458,8 @@
       <c r="D103" s="4">
         <v>543.84344924153538</v>
       </c>
-      <c r="E103" s="3">
-        <v>8</v>
+      <c r="E103" s="6">
+        <v>12</v>
       </c>
       <c r="F103" s="6">
         <v>0.95431251222908031</v>
@@ -2478,8 +2478,8 @@
       <c r="D104" s="4">
         <v>544.76380749487271</v>
       </c>
-      <c r="E104" s="3">
-        <v>8</v>
+      <c r="E104" s="6">
+        <v>12</v>
       </c>
       <c r="F104" s="6">
         <v>0.92035825333732646</v>
@@ -2498,8 +2498,8 @@
       <c r="D105" s="4">
         <v>545.64842043987574</v>
       </c>
-      <c r="E105" s="3">
-        <v>8</v>
+      <c r="E105" s="6">
+        <v>12</v>
       </c>
       <c r="F105" s="6">
         <v>0.88461294500302756</v>
@@ -2518,8 +2518,8 @@
       <c r="D106" s="4">
         <v>546.49594680383143</v>
       </c>
-      <c r="E106" s="3">
-        <v>8</v>
+      <c r="E106" s="6">
+        <v>12</v>
       </c>
       <c r="F106" s="6">
         <v>0.84752636395569425</v>
@@ -2538,8 +2538,8 @@
       <c r="D107" s="4">
         <v>547.30556555283238</v>
       </c>
-      <c r="E107" s="3">
-        <v>8</v>
+      <c r="E107" s="6">
+        <v>12</v>
       </c>
       <c r="F107" s="6">
         <v>0.80961874900094699</v>
@@ -2558,8 +2558,8 @@
       <c r="D108" s="4">
         <v>548.07705039452685</v>
       </c>
-      <c r="E108" s="3">
-        <v>8</v>
+      <c r="E108" s="6">
+        <v>12</v>
       </c>
       <c r="F108" s="6">
         <v>0.77148484169447329</v>
@@ -2578,8 +2578,8 @@
       <c r="D109" s="4">
         <v>548.81084841503161</v>
       </c>
-      <c r="E109" s="3">
-        <v>8</v>
+      <c r="E109" s="6">
+        <v>12</v>
       </c>
       <c r="F109" s="6">
         <v>0.73379802050476428</v>
@@ -2598,10 +2598,1210 @@
       <c r="D110" s="4">
         <v>549.50816293253138</v>
       </c>
-      <c r="E110" s="3">
+      <c r="E110" s="6">
+        <v>12</v>
+      </c>
+      <c r="F110" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>181</v>
+      </c>
+      <c r="B111" s="3">
+        <v>1</v>
+      </c>
+      <c r="C111" s="4">
+        <v>3483.4329999999995</v>
+      </c>
+      <c r="D111" s="4">
+        <v>595</v>
+      </c>
+      <c r="E111" s="6">
+        <v>12</v>
+      </c>
+      <c r="F111" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>182</v>
+      </c>
+      <c r="B112" s="3">
+        <v>2</v>
+      </c>
+      <c r="C112" s="4">
+        <v>3502.2899999999995</v>
+      </c>
+      <c r="D112" s="4">
+        <v>595</v>
+      </c>
+      <c r="E112" s="6">
+        <v>12</v>
+      </c>
+      <c r="F112" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
+        <v>183</v>
+      </c>
+      <c r="B113" s="3">
+        <v>3</v>
+      </c>
+      <c r="C113" s="4">
+        <v>3521.1469999999995</v>
+      </c>
+      <c r="D113" s="4">
+        <v>595</v>
+      </c>
+      <c r="E113" s="6">
+        <v>12</v>
+      </c>
+      <c r="F113" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>184</v>
+      </c>
+      <c r="B114" s="3">
+        <v>4</v>
+      </c>
+      <c r="C114" s="4">
+        <v>3540.0039999999999</v>
+      </c>
+      <c r="D114" s="4">
+        <v>595</v>
+      </c>
+      <c r="E114" s="6">
+        <v>12</v>
+      </c>
+      <c r="F114" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>185</v>
+      </c>
+      <c r="B115" s="3">
+        <v>5</v>
+      </c>
+      <c r="C115" s="4">
+        <v>3558.8609999999999</v>
+      </c>
+      <c r="D115" s="4">
+        <v>595</v>
+      </c>
+      <c r="E115" s="6">
+        <v>12</v>
+      </c>
+      <c r="F115" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>186</v>
+      </c>
+      <c r="B116" s="3">
+        <v>6</v>
+      </c>
+      <c r="C116" s="4">
+        <v>3577.7179999999998</v>
+      </c>
+      <c r="D116" s="4">
+        <v>595</v>
+      </c>
+      <c r="E116" s="6">
+        <v>12</v>
+      </c>
+      <c r="F116" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>187</v>
+      </c>
+      <c r="B117" s="3">
+        <v>7</v>
+      </c>
+      <c r="C117" s="4">
+        <v>3596.5749999999998</v>
+      </c>
+      <c r="D117" s="4">
+        <v>595</v>
+      </c>
+      <c r="E117" s="6">
+        <v>12</v>
+      </c>
+      <c r="F117" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
+        <v>188</v>
+      </c>
+      <c r="B118" s="3">
         <v>8</v>
       </c>
-      <c r="F110" s="6">
+      <c r="C118" s="4">
+        <v>3615.4319999999998</v>
+      </c>
+      <c r="D118" s="4">
+        <v>595</v>
+      </c>
+      <c r="E118" s="6">
+        <v>12</v>
+      </c>
+      <c r="F118" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="3">
+        <v>189</v>
+      </c>
+      <c r="B119" s="3">
+        <v>9</v>
+      </c>
+      <c r="C119" s="4">
+        <v>3634.2889999999998</v>
+      </c>
+      <c r="D119" s="4">
+        <v>595</v>
+      </c>
+      <c r="E119" s="6">
+        <v>12</v>
+      </c>
+      <c r="F119" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="3">
+        <v>190</v>
+      </c>
+      <c r="B120" s="3">
+        <v>10</v>
+      </c>
+      <c r="C120" s="4">
+        <v>3653.1459999999997</v>
+      </c>
+      <c r="D120" s="4">
+        <v>595</v>
+      </c>
+      <c r="E120" s="6">
+        <v>12</v>
+      </c>
+      <c r="F120" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
+        <v>191</v>
+      </c>
+      <c r="B121" s="3">
+        <v>11</v>
+      </c>
+      <c r="C121" s="4">
+        <v>3672.0029999999997</v>
+      </c>
+      <c r="D121" s="4">
+        <v>595</v>
+      </c>
+      <c r="E121" s="6">
+        <v>12</v>
+      </c>
+      <c r="F121" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
+        <v>192</v>
+      </c>
+      <c r="B122" s="3">
+        <v>12</v>
+      </c>
+      <c r="C122" s="4">
+        <v>3690.8599999999997</v>
+      </c>
+      <c r="D122" s="4">
+        <v>595</v>
+      </c>
+      <c r="E122" s="6">
+        <v>12</v>
+      </c>
+      <c r="F122" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
+        <v>193</v>
+      </c>
+      <c r="B123" s="3">
+        <v>13</v>
+      </c>
+      <c r="C123" s="4">
+        <v>3709.7169999999996</v>
+      </c>
+      <c r="D123" s="4">
+        <v>595</v>
+      </c>
+      <c r="E123" s="6">
+        <v>12</v>
+      </c>
+      <c r="F123" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
+        <v>194</v>
+      </c>
+      <c r="B124" s="3">
+        <v>14</v>
+      </c>
+      <c r="C124" s="4">
+        <v>3728.5739999999996</v>
+      </c>
+      <c r="D124" s="4">
+        <v>595</v>
+      </c>
+      <c r="E124" s="6">
+        <v>12</v>
+      </c>
+      <c r="F124" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
+        <v>195</v>
+      </c>
+      <c r="B125" s="3">
+        <v>15</v>
+      </c>
+      <c r="C125" s="4">
+        <v>3747.4309999999996</v>
+      </c>
+      <c r="D125" s="4">
+        <v>595</v>
+      </c>
+      <c r="E125" s="6">
+        <v>12</v>
+      </c>
+      <c r="F125" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="3">
+        <v>196</v>
+      </c>
+      <c r="B126" s="3">
+        <v>16</v>
+      </c>
+      <c r="C126" s="4">
+        <v>3766.2879999999996</v>
+      </c>
+      <c r="D126" s="4">
+        <v>595</v>
+      </c>
+      <c r="E126" s="6">
+        <v>12</v>
+      </c>
+      <c r="F126" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="3">
+        <v>197</v>
+      </c>
+      <c r="B127" s="3">
+        <v>17</v>
+      </c>
+      <c r="C127" s="4">
+        <v>3785.1449999999995</v>
+      </c>
+      <c r="D127" s="4">
+        <v>595</v>
+      </c>
+      <c r="E127" s="6">
+        <v>12</v>
+      </c>
+      <c r="F127" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="3">
+        <v>198</v>
+      </c>
+      <c r="B128" s="3">
+        <v>18</v>
+      </c>
+      <c r="C128" s="4">
+        <v>3804.0019999999995</v>
+      </c>
+      <c r="D128" s="4">
+        <v>595</v>
+      </c>
+      <c r="E128" s="6">
+        <v>12</v>
+      </c>
+      <c r="F128" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="3">
+        <v>199</v>
+      </c>
+      <c r="B129" s="3">
+        <v>19</v>
+      </c>
+      <c r="C129" s="4">
+        <v>3822.8589999999995</v>
+      </c>
+      <c r="D129" s="4">
+        <v>595</v>
+      </c>
+      <c r="E129" s="6">
+        <v>12</v>
+      </c>
+      <c r="F129" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="3">
+        <v>200</v>
+      </c>
+      <c r="B130" s="3">
+        <v>20</v>
+      </c>
+      <c r="C130" s="4">
+        <v>3841.7159999999994</v>
+      </c>
+      <c r="D130" s="4">
+        <v>595</v>
+      </c>
+      <c r="E130" s="6">
+        <v>12</v>
+      </c>
+      <c r="F130" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="3">
+        <v>201</v>
+      </c>
+      <c r="B131" s="3">
+        <v>21</v>
+      </c>
+      <c r="C131" s="4">
+        <v>3860.5729999999999</v>
+      </c>
+      <c r="D131" s="4">
+        <v>595</v>
+      </c>
+      <c r="E131" s="6">
+        <v>12</v>
+      </c>
+      <c r="F131" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
+        <v>202</v>
+      </c>
+      <c r="B132" s="3">
+        <v>22</v>
+      </c>
+      <c r="C132" s="4">
+        <v>3879.43</v>
+      </c>
+      <c r="D132" s="4">
+        <v>595</v>
+      </c>
+      <c r="E132" s="6">
+        <v>12</v>
+      </c>
+      <c r="F132" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="3">
+        <v>203</v>
+      </c>
+      <c r="B133" s="3">
+        <v>23</v>
+      </c>
+      <c r="C133" s="4">
+        <v>3898.2869999999998</v>
+      </c>
+      <c r="D133" s="4">
+        <v>595</v>
+      </c>
+      <c r="E133" s="6">
+        <v>12</v>
+      </c>
+      <c r="F133" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="3">
+        <v>204</v>
+      </c>
+      <c r="B134" s="3">
+        <v>24</v>
+      </c>
+      <c r="C134" s="4">
+        <v>3917.1439999999998</v>
+      </c>
+      <c r="D134" s="4">
+        <v>595</v>
+      </c>
+      <c r="E134" s="6">
+        <v>12</v>
+      </c>
+      <c r="F134" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="3">
+        <v>205</v>
+      </c>
+      <c r="B135" s="3">
+        <v>25</v>
+      </c>
+      <c r="C135" s="4">
+        <v>3936.0009999999997</v>
+      </c>
+      <c r="D135" s="4">
+        <v>595</v>
+      </c>
+      <c r="E135" s="6">
+        <v>12</v>
+      </c>
+      <c r="F135" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="3">
+        <v>206</v>
+      </c>
+      <c r="B136" s="3">
+        <v>26</v>
+      </c>
+      <c r="C136" s="4">
+        <v>3954.8579999999997</v>
+      </c>
+      <c r="D136" s="4">
+        <v>595</v>
+      </c>
+      <c r="E136" s="6">
+        <v>12</v>
+      </c>
+      <c r="F136" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="3">
+        <v>207</v>
+      </c>
+      <c r="B137" s="3">
+        <v>27</v>
+      </c>
+      <c r="C137" s="4">
+        <v>3973.7149999999997</v>
+      </c>
+      <c r="D137" s="4">
+        <v>595</v>
+      </c>
+      <c r="E137" s="6">
+        <v>12</v>
+      </c>
+      <c r="F137" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>208</v>
+      </c>
+      <c r="B138" s="3">
+        <v>28</v>
+      </c>
+      <c r="C138" s="4">
+        <v>3992.5719999999997</v>
+      </c>
+      <c r="D138" s="4">
+        <v>595</v>
+      </c>
+      <c r="E138" s="6">
+        <v>12</v>
+      </c>
+      <c r="F138" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="3">
+        <v>209</v>
+      </c>
+      <c r="B139" s="3">
+        <v>29</v>
+      </c>
+      <c r="C139" s="4">
+        <v>4011.4289999999996</v>
+      </c>
+      <c r="D139" s="4">
+        <v>595</v>
+      </c>
+      <c r="E139" s="6">
+        <v>12</v>
+      </c>
+      <c r="F139" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="3">
+        <v>210</v>
+      </c>
+      <c r="B140" s="3">
+        <v>30</v>
+      </c>
+      <c r="C140" s="4">
+        <v>4030.2859999999996</v>
+      </c>
+      <c r="D140" s="4">
+        <v>595</v>
+      </c>
+      <c r="E140" s="6">
+        <v>12</v>
+      </c>
+      <c r="F140" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="3">
+        <v>211</v>
+      </c>
+      <c r="B141" s="3">
+        <v>31</v>
+      </c>
+      <c r="C141" s="4">
+        <v>4049.1429999999996</v>
+      </c>
+      <c r="D141" s="4">
+        <v>595</v>
+      </c>
+      <c r="E141" s="6">
+        <v>12</v>
+      </c>
+      <c r="F141" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="3">
+        <v>212</v>
+      </c>
+      <c r="B142" s="3">
+        <v>32</v>
+      </c>
+      <c r="C142" s="4">
+        <v>4067.9999999999995</v>
+      </c>
+      <c r="D142" s="4">
+        <v>595</v>
+      </c>
+      <c r="E142" s="6">
+        <v>12</v>
+      </c>
+      <c r="F142" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="3">
+        <v>213</v>
+      </c>
+      <c r="B143" s="3">
+        <v>33</v>
+      </c>
+      <c r="C143" s="4">
+        <v>4086.8569999999995</v>
+      </c>
+      <c r="D143" s="4">
+        <v>595</v>
+      </c>
+      <c r="E143" s="6">
+        <v>12</v>
+      </c>
+      <c r="F143" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="3">
+        <v>214</v>
+      </c>
+      <c r="B144" s="3">
+        <v>34</v>
+      </c>
+      <c r="C144" s="4">
+        <v>4105.7139999999999</v>
+      </c>
+      <c r="D144" s="4">
+        <v>595</v>
+      </c>
+      <c r="E144" s="6">
+        <v>12</v>
+      </c>
+      <c r="F144" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="3">
+        <v>215</v>
+      </c>
+      <c r="B145" s="3">
+        <v>35</v>
+      </c>
+      <c r="C145" s="4">
+        <v>4124.5709999999999</v>
+      </c>
+      <c r="D145" s="4">
+        <v>595</v>
+      </c>
+      <c r="E145" s="6">
+        <v>12</v>
+      </c>
+      <c r="F145" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="3">
+        <v>216</v>
+      </c>
+      <c r="B146" s="3">
+        <v>36</v>
+      </c>
+      <c r="C146" s="4">
+        <v>4143.4279999999999</v>
+      </c>
+      <c r="D146" s="4">
+        <v>595</v>
+      </c>
+      <c r="E146" s="6">
+        <v>12</v>
+      </c>
+      <c r="F146" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="3">
+        <v>217</v>
+      </c>
+      <c r="B147" s="3">
+        <v>37</v>
+      </c>
+      <c r="C147" s="4">
+        <v>4162.2849999999999</v>
+      </c>
+      <c r="D147" s="4">
+        <v>595</v>
+      </c>
+      <c r="E147" s="6">
+        <v>12</v>
+      </c>
+      <c r="F147" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="3">
+        <v>218</v>
+      </c>
+      <c r="B148" s="3">
+        <v>38</v>
+      </c>
+      <c r="C148" s="4">
+        <v>4181.1419999999998</v>
+      </c>
+      <c r="D148" s="4">
+        <v>595</v>
+      </c>
+      <c r="E148" s="6">
+        <v>12</v>
+      </c>
+      <c r="F148" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
+        <v>219</v>
+      </c>
+      <c r="B149" s="3">
+        <v>39</v>
+      </c>
+      <c r="C149" s="4">
+        <v>4199.9989999999998</v>
+      </c>
+      <c r="D149" s="4">
+        <v>595</v>
+      </c>
+      <c r="E149" s="6">
+        <v>12</v>
+      </c>
+      <c r="F149" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="3">
+        <v>220</v>
+      </c>
+      <c r="B150" s="3">
+        <v>40</v>
+      </c>
+      <c r="C150" s="4">
+        <v>4218.8559999999998</v>
+      </c>
+      <c r="D150" s="4">
+        <v>595</v>
+      </c>
+      <c r="E150" s="6">
+        <v>12</v>
+      </c>
+      <c r="F150" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="3">
+        <v>221</v>
+      </c>
+      <c r="B151" s="3">
+        <v>41</v>
+      </c>
+      <c r="C151" s="4">
+        <v>4237.7129999999997</v>
+      </c>
+      <c r="D151" s="4">
+        <v>595</v>
+      </c>
+      <c r="E151" s="6">
+        <v>12</v>
+      </c>
+      <c r="F151" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="3">
+        <v>222</v>
+      </c>
+      <c r="B152" s="3">
+        <v>42</v>
+      </c>
+      <c r="C152" s="4">
+        <v>4256.57</v>
+      </c>
+      <c r="D152" s="4">
+        <v>595</v>
+      </c>
+      <c r="E152" s="6">
+        <v>12</v>
+      </c>
+      <c r="F152" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="3">
+        <v>223</v>
+      </c>
+      <c r="B153" s="3">
+        <v>43</v>
+      </c>
+      <c r="C153" s="4">
+        <v>4275.4269999999997</v>
+      </c>
+      <c r="D153" s="4">
+        <v>595</v>
+      </c>
+      <c r="E153" s="6">
+        <v>12</v>
+      </c>
+      <c r="F153" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="3">
+        <v>224</v>
+      </c>
+      <c r="B154" s="3">
+        <v>44</v>
+      </c>
+      <c r="C154" s="4">
+        <v>4294.2839999999997</v>
+      </c>
+      <c r="D154" s="4">
+        <v>595</v>
+      </c>
+      <c r="E154" s="6">
+        <v>12</v>
+      </c>
+      <c r="F154" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="3">
+        <v>225</v>
+      </c>
+      <c r="B155" s="3">
+        <v>45</v>
+      </c>
+      <c r="C155" s="4">
+        <v>4313.1409999999996</v>
+      </c>
+      <c r="D155" s="4">
+        <v>595</v>
+      </c>
+      <c r="E155" s="6">
+        <v>12</v>
+      </c>
+      <c r="F155" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="3">
+        <v>226</v>
+      </c>
+      <c r="B156" s="3">
+        <v>46</v>
+      </c>
+      <c r="C156" s="4">
+        <v>4331.9979999999996</v>
+      </c>
+      <c r="D156" s="4">
+        <v>595</v>
+      </c>
+      <c r="E156" s="6">
+        <v>12</v>
+      </c>
+      <c r="F156" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" s="3">
+        <v>227</v>
+      </c>
+      <c r="B157" s="3">
+        <v>47</v>
+      </c>
+      <c r="C157" s="4">
+        <v>4350.8549999999996</v>
+      </c>
+      <c r="D157" s="4">
+        <v>595</v>
+      </c>
+      <c r="E157" s="6">
+        <v>12</v>
+      </c>
+      <c r="F157" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="3">
+        <v>228</v>
+      </c>
+      <c r="B158" s="3">
+        <v>48</v>
+      </c>
+      <c r="C158" s="4">
+        <v>4369.7119999999995</v>
+      </c>
+      <c r="D158" s="4">
+        <v>595</v>
+      </c>
+      <c r="E158" s="6">
+        <v>12</v>
+      </c>
+      <c r="F158" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="3">
+        <v>229</v>
+      </c>
+      <c r="B159" s="3">
+        <v>49</v>
+      </c>
+      <c r="C159" s="4">
+        <v>4388.5689999999995</v>
+      </c>
+      <c r="D159" s="4">
+        <v>595</v>
+      </c>
+      <c r="E159" s="6">
+        <v>12</v>
+      </c>
+      <c r="F159" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="3">
+        <v>230</v>
+      </c>
+      <c r="B160" s="3">
+        <v>50</v>
+      </c>
+      <c r="C160" s="4">
+        <v>4407.4259999999995</v>
+      </c>
+      <c r="D160" s="4">
+        <v>595</v>
+      </c>
+      <c r="E160" s="6">
+        <v>12</v>
+      </c>
+      <c r="F160" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" s="3">
+        <v>231</v>
+      </c>
+      <c r="B161" s="3">
+        <v>51</v>
+      </c>
+      <c r="C161" s="4">
+        <v>4426.2829999999994</v>
+      </c>
+      <c r="D161" s="4">
+        <v>595</v>
+      </c>
+      <c r="E161" s="6">
+        <v>12</v>
+      </c>
+      <c r="F161" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" s="3">
+        <v>232</v>
+      </c>
+      <c r="B162" s="3">
+        <v>52</v>
+      </c>
+      <c r="C162" s="4">
+        <v>4445.1399999999994</v>
+      </c>
+      <c r="D162" s="4">
+        <v>595</v>
+      </c>
+      <c r="E162" s="6">
+        <v>12</v>
+      </c>
+      <c r="F162" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" s="3">
+        <v>233</v>
+      </c>
+      <c r="B163" s="3">
+        <v>53</v>
+      </c>
+      <c r="C163" s="4">
+        <v>4463.9969999999994</v>
+      </c>
+      <c r="D163" s="4">
+        <v>595</v>
+      </c>
+      <c r="E163" s="6">
+        <v>12</v>
+      </c>
+      <c r="F163" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" s="3">
+        <v>234</v>
+      </c>
+      <c r="B164" s="3">
+        <v>54</v>
+      </c>
+      <c r="C164" s="4">
+        <v>4482.8539999999994</v>
+      </c>
+      <c r="D164" s="4">
+        <v>595</v>
+      </c>
+      <c r="E164" s="6">
+        <v>12</v>
+      </c>
+      <c r="F164" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" s="3">
+        <v>235</v>
+      </c>
+      <c r="B165" s="3">
+        <v>55</v>
+      </c>
+      <c r="C165" s="4">
+        <v>4501.7109999999993</v>
+      </c>
+      <c r="D165" s="4">
+        <v>595</v>
+      </c>
+      <c r="E165" s="6">
+        <v>12</v>
+      </c>
+      <c r="F165" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" s="3">
+        <v>236</v>
+      </c>
+      <c r="B166" s="3">
+        <v>56</v>
+      </c>
+      <c r="C166" s="4">
+        <v>4520.5679999999993</v>
+      </c>
+      <c r="D166" s="4">
+        <v>595</v>
+      </c>
+      <c r="E166" s="6">
+        <v>12</v>
+      </c>
+      <c r="F166" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" s="3">
+        <v>237</v>
+      </c>
+      <c r="B167" s="3">
+        <v>57</v>
+      </c>
+      <c r="C167" s="4">
+        <v>4539.4249999999993</v>
+      </c>
+      <c r="D167" s="4">
+        <v>595</v>
+      </c>
+      <c r="E167" s="6">
+        <v>12</v>
+      </c>
+      <c r="F167" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" s="3">
+        <v>238</v>
+      </c>
+      <c r="B168" s="3">
+        <v>58</v>
+      </c>
+      <c r="C168" s="4">
+        <v>4558.2819999999992</v>
+      </c>
+      <c r="D168" s="4">
+        <v>595</v>
+      </c>
+      <c r="E168" s="6">
+        <v>12</v>
+      </c>
+      <c r="F168" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169" s="3">
+        <v>239</v>
+      </c>
+      <c r="B169" s="3">
+        <v>59</v>
+      </c>
+      <c r="C169" s="4">
+        <v>4577.1389999999992</v>
+      </c>
+      <c r="D169" s="4">
+        <v>595</v>
+      </c>
+      <c r="E169" s="6">
+        <v>12</v>
+      </c>
+      <c r="F169" s="6">
+        <v>0.69731451749976259</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A170" s="3">
+        <v>240</v>
+      </c>
+      <c r="B170" s="3">
+        <v>60</v>
+      </c>
+      <c r="C170" s="4">
+        <v>4595.9960000000001</v>
+      </c>
+      <c r="D170" s="4">
+        <v>595</v>
+      </c>
+      <c r="E170" s="6">
+        <v>12</v>
+      </c>
+      <c r="F170" s="6">
         <v>0.69731451749976259</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update max range and account for shooter foam
</commit_message>
<xml_diff>
--- a/steamworks/conf/shooter_data.xlsx
+++ b/steamworks/conf/shooter_data.xlsx
@@ -394,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
       <selection sqref="A1:F170"/>
     </sheetView>
   </sheetViews>
@@ -436,13 +436,13 @@
         <v>1428.02</v>
       </c>
       <c r="D2" s="4">
-        <v>440.27514384998631</v>
+        <v>430.42957545556726</v>
       </c>
       <c r="E2" s="6">
         <v>8</v>
       </c>
       <c r="F2" s="6">
-        <v>0.30267915437361809</v>
+        <v>0.63358699953887476</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -456,13 +456,13 @@
         <v>1446.877</v>
       </c>
       <c r="D3" s="4">
-        <v>440.62782300435993</v>
+        <v>431.11316245510613</v>
       </c>
       <c r="E3" s="6">
         <v>8.0476190476190474</v>
       </c>
       <c r="F3" s="6">
-        <v>0.35267915437361808</v>
+        <v>0.68358699953887481</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -476,13 +476,13 @@
         <v>1465.7339999999999</v>
       </c>
       <c r="D4" s="4">
-        <v>441.02827356885882</v>
+        <v>431.8248497944486</v>
       </c>
       <c r="E4" s="6">
         <v>8.0952380952380949</v>
       </c>
       <c r="F4" s="6">
-        <v>0.40045056449889671</v>
+        <v>0.7116873393424612</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -496,13 +496,13 @@
         <v>1484.5909999999999</v>
       </c>
       <c r="D5" s="4">
-        <v>441.48299817210409</v>
+        <v>432.56342657458293</v>
       </c>
       <c r="E5" s="6">
         <v>8.1428571428571423</v>
       </c>
       <c r="F5" s="6">
-        <v>0.45472460324526764</v>
+        <v>0.7385767801343377</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -516,13 +516,13 @@
         <v>1503.4480000000001</v>
       </c>
       <c r="D6" s="4">
-        <v>441.99711144930097</v>
+        <v>433.32770991742893</v>
       </c>
       <c r="E6" s="6">
         <v>8.1904761904761898</v>
       </c>
       <c r="F6" s="6">
-        <v>0.51411327719688416</v>
+        <v>0.76428334284599941</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -536,13 +536,13 @@
         <v>1522.3050000000001</v>
       </c>
       <c r="D7" s="4">
-        <v>442.57445352221384</v>
+        <v>434.11654468790431</v>
       </c>
       <c r="E7" s="6">
         <v>8.2380952380952372</v>
       </c>
       <c r="F7" s="6">
-        <v>0.57734207291287021</v>
+        <v>0.78883477047537554</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -556,13 +556,13 @@
         <v>1541.162</v>
       </c>
       <c r="D8" s="4">
-        <v>443.21769866434897</v>
+        <v>434.92880321599176</v>
       </c>
       <c r="E8" s="6">
         <v>8.2857142857142847</v>
       </c>
       <c r="F8" s="6">
-        <v>0.64324514213512884</v>
+        <v>0.81225852808745458</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -576,13 +576,13 @@
         <v>1560.019</v>
       </c>
       <c r="D9" s="4">
-        <v>443.92845923987898</v>
+        <v>435.76338501880599</v>
       </c>
       <c r="E9" s="6">
         <v>8.3333333333333321</v>
       </c>
       <c r="F9" s="6">
-        <v>0.71076057553000282</v>
+        <v>0.83458180281422756</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -596,13 +596,13 @@
         <v>1578.876</v>
       </c>
       <c r="D10" s="4">
-        <v>444.70738500496645</v>
+        <v>436.61921652266039</v>
       </c>
       <c r="E10" s="6">
         <v>8.3809523809523796</v>
       </c>
       <c r="F10" s="6">
-        <v>0.77892576508747879</v>
+        <v>0.85583150385440376</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -616,13 +616,13 @@
         <v>1597.7329999999999</v>
       </c>
       <c r="D11" s="4">
-        <v>445.55425785993339</v>
+        <v>437.49525078513483</v>
       </c>
       <c r="E11" s="6">
         <v>8.428571428571427</v>
       </c>
       <c r="F11" s="6">
-        <v>0.84687285496693221</v>
+        <v>0.87603426247443394</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -636,13 +636,13 @@
         <v>1616.59</v>
       </c>
       <c r="D12" s="4">
-        <v>446.46808214099929</v>
+        <v>438.39046721714135</v>
       </c>
       <c r="E12" s="6">
         <v>8.4761904761904745</v>
       </c>
       <c r="F12" s="6">
-        <v>0.91382428106589941</v>
+        <v>0.89521643200652079</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -656,13 +656,13 @@
         <v>1635.4469999999999</v>
       </c>
       <c r="D13" s="4">
-        <v>447.44717054000557</v>
+        <v>439.30387130499173</v>
       </c>
       <c r="E13" s="6">
         <v>8.5238095238095219</v>
       </c>
       <c r="F13" s="6">
-        <v>0.97908839900628664</v>
+        <v>0.91340408785038107</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -676,13 +676,13 @@
         <v>1654.3039999999999</v>
       </c>
       <c r="D14" s="4">
-        <v>448.48922574087464</v>
+        <v>440.23449433246424</v>
       </c>
       <c r="E14" s="6">
         <v>8.5714285714285694</v>
       </c>
       <c r="F14" s="6">
-        <v>1.042055200869072</v>
+        <v>0.93062302747250669</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -696,13 +696,13 @@
         <v>1673.1610000000001</v>
       </c>
       <c r="D15" s="4">
-        <v>449.59141786130476</v>
+        <v>441.18139310287097</v>
       </c>
       <c r="E15" s="6">
         <v>8.6190476190476168</v>
       </c>
       <c r="F15" s="6">
-        <v>1.1021921204301179</v>
+        <v>0.94689877040673309</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -716,13 +716,13 @@
         <v>1692.018</v>
       </c>
       <c r="D16" s="4">
-        <v>450.75045778817275</v>
+        <v>442.1436496611247</v>
       </c>
       <c r="E16" s="6">
         <v>8.6666666666666643</v>
       </c>
       <c r="F16" s="6">
-        <v>1.1590399268679903</v>
+        <v>0.96225655825372769</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -736,13 +736,13 @@
         <v>1710.875</v>
       </c>
       <c r="D17" s="4">
-        <v>451.96266649545123</v>
+        <v>443.12037101580466</v>
       </c>
       <c r="E17" s="6">
         <v>8.7142857142857117</v>
       </c>
       <c r="F17" s="6">
-        <v>1.212208707278478</v>
+        <v>0.97672135467996668</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -756,13 +756,13 @@
         <v>1729.732</v>
       </c>
       <c r="D18" s="4">
-        <v>453.22404043302868</v>
+        <v>444.11068886122536</v>
       </c>
       <c r="E18" s="6">
         <v>8.7619047619047592</v>
       </c>
       <c r="F18" s="6">
-        <v>1.2613739375774458</v>
+        <v>0.9903178454206909</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -776,13 +776,13 @@
         <v>1748.5889999999999</v>
       </c>
       <c r="D19" s="4">
-        <v>454.53031307500987</v>
+        <v>445.11375929950168</v>
       </c>
       <c r="E19" s="6">
         <v>8.8095238095238066</v>
       </c>
       <c r="F19" s="6">
-        <v>1.3062726419811952</v>
+        <v>1.0030704382763247</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -796,13 +796,13 @@
         <v>1767.4459999999999</v>
       </c>
       <c r="D20" s="4">
-        <v>455.8770127163798</v>
+        <v>446.12876256261734</v>
       </c>
       <c r="E20" s="6">
         <v>8.8571428571428541</v>
       </c>
       <c r="F20" s="6">
-        <v>1.3466996413699235</v>
+        <v>1.0150032631156591</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -816,13 +816,13 @@
         <v>1786.3029999999999</v>
       </c>
       <c r="D21" s="4">
-        <v>457.25951660599367</v>
+        <v>447.15490273449092</v>
       </c>
       <c r="E21" s="6">
         <v>8.9047619047619015</v>
       </c>
       <c r="F21" s="6">
-        <v>1.3825038896138722</v>
+        <v>1.0261401718735783</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -836,13 +836,13 @@
         <v>1805.16</v>
       </c>
       <c r="D22" s="4">
-        <v>458.67310150524554</v>
+        <v>448.19140747304306</v>
       </c>
       <c r="E22" s="6">
         <v>8.952380952380949</v>
       </c>
       <c r="F22" s="6">
-        <v>1.4135848992518731</v>
+        <v>1.0365047385521393</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -856,13 +856,13 @@
         <v>1824.0170000000001</v>
       </c>
       <c r="D23" s="4">
-        <v>460.11299076028354</v>
+        <v>449.23752773226272</v>
       </c>
       <c r="E23" s="6">
         <v>8.9999999999999964</v>
       </c>
       <c r="F23" s="6">
-        <v>1.4398892550379969</v>
+        <v>1.0461202592196628</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -876,13 +876,13 @@
         <v>1842.874</v>
       </c>
       <c r="D24" s="4">
-        <v>461.57439797681855</v>
+        <v>450.2925374842755</v>
       </c>
       <c r="E24" s="6">
         <v>9.0476190476190439</v>
       </c>
       <c r="F24" s="6">
-        <v>1.461407216535008</v>
+        <v>1.0550097520127792</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -896,13 +896,13 @@
         <v>1861.731</v>
       </c>
       <c r="D25" s="4">
-        <v>463.05256738591834</v>
+        <v>451.35573344140948</v>
       </c>
       <c r="E25" s="6">
         <v>9.0952380952380913</v>
       </c>
       <c r="F25" s="6">
-        <v>1.4781694090997917</v>
+        <v>1.0631959571339848</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -916,13 +916,13 @@
         <v>1880.588</v>
       </c>
       <c r="D26" s="4">
-        <v>464.54281098940828</v>
+        <v>452.42643477826266</v>
       </c>
       <c r="E26" s="6">
         <v>9.1428571428571388</v>
       </c>
       <c r="F26" s="6">
-        <v>1.4902436034899438</v>
+        <v>1.0707013368531761</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -936,13 +936,13 @@
         <v>1899.4449999999999</v>
       </c>
       <c r="D27" s="4">
-        <v>466.04054257343068</v>
+        <v>453.503982853769</v>
       </c>
       <c r="E27" s="6">
         <v>9.1904761904761862</v>
       </c>
       <c r="F27" s="6">
-        <v>1.4977315840224037</v>
+        <v>1.0775480755063427</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -956,13 +956,13 @@
         <v>1918.3019999999999</v>
       </c>
       <c r="D28" s="4">
-        <v>467.54130867869662</v>
+        <v>454.58774093326679</v>
       </c>
       <c r="E28" s="6">
         <v>9.2380952380952337</v>
       </c>
       <c r="F28" s="6">
-        <v>1.5007661052659387</v>
+        <v>1.0837580794977839</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -976,13 +976,13 @@
         <v>1937.1589999999999</v>
       </c>
       <c r="D29" s="4">
-        <v>469.04081661616055</v>
+        <v>455.67709391056417</v>
       </c>
       <c r="E29" s="6">
         <v>9.2857142857142811</v>
       </c>
       <c r="F29" s="6">
-        <v>1.4995079374639317</v>
+        <v>1.0893529772973807</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -996,13 +996,13 @@
         <v>1956.0159999999998</v>
       </c>
       <c r="D30" s="4">
-        <v>470.53495961657154</v>
+        <v>456.77144803000738</v>
       </c>
       <c r="E30" s="6">
         <v>9.3333333333333286</v>
       </c>
       <c r="F30" s="6">
-        <v>1.4941430004109861</v>
+        <v>1.09435411944321</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1016,13 +1016,13 @@
         <v>1974.873</v>
       </c>
       <c r="D31" s="4">
-        <v>472.01983920236944</v>
+        <v>457.87023060854642</v>
       </c>
       <c r="E31" s="6">
         <v>9.380952380952376</v>
       </c>
       <c r="F31" s="6">
-        <v>1.4848795857978985</v>
+        <v>1.0987825785390442</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1036,13 +1036,13 @@
         <v>1993.73</v>
       </c>
       <c r="D32" s="4">
-        <v>473.49178487111476</v>
+        <v>458.97288975780248</v>
       </c>
       <c r="E32" s="6">
         <v>9.4285714285714235</v>
       </c>
       <c r="F32" s="6">
-        <v>1.4719456687453203</v>
+        <v>1.1026591492560556</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1056,13 +1056,13 @@
         <v>2012.587</v>
       </c>
       <c r="D33" s="4">
-        <v>474.94737117773457</v>
+        <v>460.07889410613552</v>
       </c>
       <c r="E33" s="6">
         <v>9.4761904761904709</v>
       </c>
       <c r="F33" s="6">
-        <v>1.4555863066198071</v>
+        <v>1.1060043483330446</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1076,13 +1076,13 @@
         <v>2031.444</v>
       </c>
       <c r="D34" s="4">
-        <v>476.38343230588634</v>
+        <v>461.18773252071003</v>
       </c>
       <c r="E34" s="6">
         <v>9.5238095238095184</v>
       </c>
       <c r="F34" s="6">
-        <v>1.4360611281517777</v>
+        <v>1.1088384145745067</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1096,13 +1096,13 @@
         <v>2050.3009999999999</v>
       </c>
       <c r="D35" s="4">
-        <v>477.79707421544572</v>
+        <v>462.29891382956293</v>
       </c>
       <c r="E35" s="6">
         <v>9.5714285714285658</v>
       </c>
       <c r="F35" s="6">
-        <v>1.4136419095593737</v>
+        <v>1.1111813088529061</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1116,13 +1116,13 @@
         <v>2069.1579999999999</v>
       </c>
       <c r="D36" s="4">
-        <v>479.18568445575056</v>
+        <v>463.41196654367002</v>
       </c>
       <c r="E36" s="6">
         <v>9.6190476190476133</v>
       </c>
       <c r="F36" s="6">
-        <v>1.3886102403048426</v>
+        <v>1.1130527141070843</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1136,13 +1136,13 @@
         <v>2088.0149999999999</v>
       </c>
       <c r="D37" s="4">
-        <v>480.54693973269877</v>
+        <v>464.52643857901239</v>
       </c>
       <c r="E37" s="6">
         <v>9.6666666666666607</v>
       </c>
       <c r="F37" s="6">
-        <v>1.3612552769482136</v>
+        <v>1.1144720353423736</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1156,13 +1156,13 @@
         <v>2106.8719999999998</v>
       </c>
       <c r="D38" s="4">
-        <v>481.87881131825543</v>
+        <v>465.64189697864481</v>
       </c>
       <c r="E38" s="6">
         <v>9.7142857142857082</v>
       </c>
       <c r="F38" s="6">
-        <v>1.3318715855566552</v>
+        <v>1.1154583996324163</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1176,13 +1176,13 @@
         <v>2125.7289999999998</v>
       </c>
       <c r="D39" s="4">
-        <v>483.17956839119415</v>
+        <v>466.75792763476136</v>
       </c>
       <c r="E39" s="6">
         <v>9.7619047619047556</v>
       </c>
       <c r="F39" s="6">
-        <v>1.3007570729387226</v>
+        <v>1.1160306561165498</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1196,13 +1196,13 @@
         <v>2144.5859999999998</v>
       </c>
       <c r="D40" s="4">
-        <v>484.44777939768665</v>
+        <v>467.87413501076298</v>
       </c>
       <c r="E40" s="6">
         <v>9.8095238095238031</v>
       </c>
       <c r="F40" s="6">
-        <v>1.2682110064924927</v>
+        <v>1.1162073760016256</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1216,13 +1216,13 @@
         <v>2163.4429999999998</v>
       </c>
       <c r="D41" s="4">
-        <v>485.68231151964119</v>
+        <v>468.99014186332363</v>
       </c>
       <c r="E41" s="6">
         <v>9.8571428571428505</v>
       </c>
       <c r="F41" s="6">
-        <v>1.234532121954544</v>
+        <v>1.1160068525606448</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1236,13 +1236,13 @@
         <v>2182.2999999999997</v>
       </c>
       <c r="D42" s="4">
-        <v>486.8823283406191</v>
+        <v>470.10558896445855</v>
       </c>
       <c r="E42" s="6">
         <v>9.904761904761898</v>
       </c>
       <c r="F42" s="6">
-        <v>1.2000168209779076</v>
+        <v>1.1154471011349187</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1256,13 +1256,13 @@
         <v>2201.1569999999997</v>
       </c>
       <c r="D43" s="4">
-        <v>488.04728579644416</v>
+        <v>471.22013482358989</v>
       </c>
       <c r="E43" s="6">
         <v>9.9523809523809454</v>
       </c>
       <c r="F43" s="6">
-        <v>1.1649574558250606</v>
+        <v>1.11454585913134</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1276,13 +1276,13 @@
         <v>2220.0139999999997</v>
       </c>
       <c r="D44" s="4">
-        <v>489.17692650033405</v>
+        <v>472.33345540961432</v>
       </c>
       <c r="E44" s="6">
         <v>9.9999999999999929</v>
       </c>
       <c r="F44" s="6">
-        <v>1.1296407038898906</v>
+        <v>1.1133205860244288</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1296,13 +1296,13 @@
         <v>2238.8709999999996</v>
       </c>
       <c r="D45" s="4">
-        <v>490.27127253045455</v>
+        <v>473.44524387297008</v>
       </c>
       <c r="E45" s="6">
         <v>10.04761904761904</v>
       </c>
       <c r="F45" s="6">
-        <v>1.094346030120505</v>
+        <v>1.1117884633557651</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1316,13 +1316,13 @@
         <v>2257.7279999999996</v>
       </c>
       <c r="D46" s="4">
-        <v>491.33061676848865</v>
+        <v>474.55521026770305</v>
       </c>
       <c r="E46" s="6">
         <v>10.095238095238088</v>
       </c>
       <c r="F46" s="6">
-        <v>1.0593442380341003</v>
+        <v>1.1099663947329645</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1336,13 +1336,13 @@
         <v>2276.5849999999996</v>
       </c>
       <c r="D47" s="4">
-        <v>492.35551287815451</v>
+        <v>475.66308127353443</v>
       </c>
       <c r="E47" s="6">
         <v>10.142857142857135</v>
       </c>
       <c r="F47" s="6">
-        <v>1.0248961096658604</v>
+        <v>1.1078710058313845</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1356,13 +1356,13 @@
         <v>2295.4419999999996</v>
       </c>
       <c r="D48" s="4">
-        <v>493.34676401189336</v>
+        <v>476.76859991792821</v>
       </c>
       <c r="E48" s="6">
         <v>10.190476190476183</v>
       </c>
       <c r="F48" s="6">
-        <v>0.99125113373884233</v>
+        <v>1.1055186443937828</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1376,13 +1376,13 @@
         <v>2314.2989999999995</v>
       </c>
       <c r="D49" s="4">
-        <v>494.30541033462487</v>
+        <v>477.87152529815626</v>
       </c>
       <c r="E49" s="6">
         <v>10.23809523809523</v>
       </c>
       <c r="F49" s="6">
-        <v>0.95864632273151074</v>
+        <v>1.1029253802280437</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1396,13 +1396,13 @@
         <v>2333.1559999999999</v>
       </c>
       <c r="D50" s="4">
-        <v>495.23271545273292</v>
+        <v>478.97163230336673</v>
       </c>
       <c r="E50" s="6">
         <v>10.285714285714278</v>
       </c>
       <c r="F50" s="6">
-        <v>0.92730511810805183</v>
+        <v>1.1001070052104751</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1416,13 +1416,13 @@
         <v>2352.0129999999999</v>
       </c>
       <c r="D51" s="4">
-        <v>496.13015183715015</v>
+        <v>480.06871133665118</v>
       </c>
       <c r="E51" s="6">
         <v>10.333333333333325</v>
       </c>
       <c r="F51" s="6">
-        <v>0.89743638441723306</v>
+        <v>1.0970790332844444</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1436,13 +1436,13 @@
         <v>2370.87</v>
       </c>
       <c r="D52" s="4">
-        <v>496.99938532943179</v>
+        <v>481.16256803711019</v>
       </c>
       <c r="E52" s="6">
         <v>10.380952380952372</v>
       </c>
       <c r="F52" s="6">
-        <v>0.86923349228163715</v>
+        <v>1.0938567004590141</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1456,13 +1456,13 @@
         <v>2389.7269999999999</v>
       </c>
       <c r="D53" s="4">
-        <v>497.84225881863949</v>
+        <v>482.25302300192152</v>
       </c>
       <c r="E53" s="6">
         <v>10.42857142857142</v>
       </c>
       <c r="F53" s="6">
-        <v>0.84287348920770455</v>
+        <v>1.0904549648113289</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1476,13 +1476,13 @@
         <v>2408.5839999999998</v>
       </c>
       <c r="D54" s="4">
-        <v>498.66077517767826</v>
+        <v>483.33991150840654</v>
       </c>
       <c r="E54" s="6">
         <v>10.476190476190467</v>
       </c>
       <c r="F54" s="6">
-        <v>0.8185163590387674</v>
+        <v>1.0868885064850247</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1496,13 +1496,13 @@
         <v>2427.4409999999998</v>
       </c>
       <c r="D55" s="4">
-        <v>499.45707954938825</v>
+        <v>484.42308323609643</v>
       </c>
       <c r="E55" s="6">
         <v>10.523809523809515</v>
       </c>
       <c r="F55" s="6">
-        <v>0.79630437170999357</v>
+        <v>1.0831717276898871</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1516,13 +1516,13 @@
         <v>2446.2979999999998</v>
       </c>
       <c r="D56" s="4">
-        <v>500.23344106768036</v>
+        <v>485.5024019888009</v>
       </c>
       <c r="E56" s="6">
         <v>10.571428571428562</v>
       </c>
       <c r="F56" s="6">
-        <v>0.77636151829210576</v>
+        <v>1.0793187527044665</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1536,13 +1536,13 @@
         <v>2465.1549999999997</v>
       </c>
       <c r="D57" s="4">
-        <v>500.99223410566174</v>
+        <v>486.57774541667334</v>
       </c>
       <c r="E57" s="6">
         <v>10.61904761904761</v>
       </c>
       <c r="F57" s="6">
-        <v>0.75879303798137698</v>
+        <v>1.0753434278724399</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -1556,13 +1556,13 @@
         <v>2484.0119999999997</v>
       </c>
       <c r="D58" s="4">
-        <v>501.73591913733526</v>
+        <v>487.64900473827868</v>
       </c>
       <c r="E58" s="6">
         <v>10.666666666666657</v>
       </c>
       <c r="F58" s="6">
-        <v>0.74368503167352173</v>
+        <v>1.0712593216053392</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -1576,13 +1576,13 @@
         <v>2502.8689999999997</v>
       </c>
       <c r="D59" s="4">
-        <v>502.46702330170501</v>
+        <v>488.71608446266021</v>
       </c>
       <c r="E59" s="6">
         <v>10.714285714285705</v>
       </c>
       <c r="F59" s="6">
-        <v>0.73110416436975356</v>
+        <v>1.0670797243815286</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -1596,13 +1596,13 @@
         <v>2521.7259999999997</v>
       </c>
       <c r="D60" s="4">
-        <v>503.18812075873848</v>
+        <v>489.77890211140607</v>
       </c>
       <c r="E60" s="6">
         <v>10.761904761904752</v>
       </c>
       <c r="F60" s="6">
-        <v>0.72109745703346562</v>
+        <v>1.0628176487458632</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -1616,13 +1616,13 @@
         <v>2540.5829999999996</v>
       </c>
       <c r="D61" s="4">
-        <v>503.90181292460602</v>
+        <v>490.83738794071689</v>
       </c>
       <c r="E61" s="6">
         <v>10.8095238095238</v>
       </c>
       <c r="F61" s="6">
-        <v>0.71369216586754192</v>
+        <v>1.0584858293108255</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -1636,13 +1636,13 @@
         <v>2559.4399999999996</v>
       </c>
       <c r="D62" s="4">
-        <v>504.61070867562648</v>
+        <v>491.89148466347194</v>
       </c>
       <c r="E62" s="6">
         <v>10.857142857142847</v>
       </c>
       <c r="F62" s="6">
-        <v>0.70889575102046365</v>
+        <v>1.0540967227550482</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -1656,13 +1656,13 @@
         <v>2578.2969999999996</v>
       </c>
       <c r="D63" s="4">
-        <v>505.31740460920537</v>
+        <v>492.94114717129696</v>
       </c>
       <c r="E63" s="6">
         <v>10.904761904761894</v>
       </c>
       <c r="F63" s="6">
-        <v>0.70669593357888516</v>
+        <v>1.049662507825019</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -1676,13 +1676,13 @@
         <v>2597.1539999999995</v>
       </c>
       <c r="D64" s="4">
-        <v>506.02446545036491</v>
+        <v>493.98634225662943</v>
       </c>
       <c r="E64" s="6">
         <v>10.952380952380942</v>
       </c>
       <c r="F64" s="6">
-        <v>0.70706084115954582</v>
+        <v>1.0451950853324661</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -1696,13 +1696,13 @@
         <v>2616.0109999999995</v>
       </c>
       <c r="D65" s="4">
-        <v>506.7344046920216</v>
+        <v>495.02704833478845</v>
       </c>
       <c r="E65" s="6">
         <v>10.999999999999989</v>
       </c>
       <c r="F65" s="6">
-        <v>0.70993924165668432</v>
+        <v>1.0407060781590189</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -1716,13 +1716,13 @@
         <v>2634.8679999999995</v>
       </c>
       <c r="D66" s="4">
-        <v>507.4496655584835</v>
+        <v>496.06325516603829</v>
       </c>
       <c r="E66" s="6">
         <v>11.047619047619037</v>
       </c>
       <c r="F66" s="6">
-        <v>0.71526086646190379</v>
+        <v>1.0362068312498423</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -1736,13 +1736,13 @@
         <v>2653.7249999999999</v>
       </c>
       <c r="D67" s="4">
-        <v>508.17260238022118</v>
+        <v>497.09496357765727</v>
       </c>
       <c r="E67" s="6">
         <v>11.095238095238084</v>
       </c>
       <c r="F67" s="6">
-        <v>0.72293682173767593</v>
+        <v>1.031708411618979</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -1756,13 +1756,13 @@
         <v>2672.5819999999999</v>
       </c>
       <c r="D68" s="4">
-        <v>508.90546246811846</v>
+        <v>498.12218518600457</v>
       </c>
       <c r="E68" s="6">
         <v>11.142857142857132</v>
       </c>
       <c r="F68" s="6">
-        <v>0.7328600878972793</v>
+        <v>1.027221608347304</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -1776,13 +1776,13 @@
         <v>2691.4389999999999</v>
       </c>
       <c r="D69" s="4">
-        <v>509.6503685766902</v>
+        <v>499.14494211858675</v>
       </c>
       <c r="E69" s="6">
         <v>11.190476190476179</v>
       </c>
       <c r="F69" s="6">
-        <v>0.74490610857174033</v>
+        <v>1.0227569325821833</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -1796,13 +1796,13 @@
         <v>2710.2959999999998</v>
       </c>
       <c r="D70" s="4">
-        <v>510.40930204362212</v>
+        <v>500.16326673612491</v>
       </c>
       <c r="E70" s="6">
         <v>11.238095238095227</v>
       </c>
       <c r="F70" s="6">
-        <v>0.75893346693192143</v>
+        <v>1.0183246175381555</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -1816,13 +1816,13 @@
         <v>2729.1529999999998</v>
       </c>
       <c r="D71" s="4">
-        <v>511.18408669597829</v>
+        <v>501.17720135462105</v>
       </c>
       <c r="E71" s="6">
         <v>11.285714285714274</v>
       </c>
       <c r="F71" s="6">
-        <v>0.77478465235617477</v>
+        <v>1.0139346184961369</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -1836,13 +1836,13 @@
         <v>2748.0099999999998</v>
       </c>
       <c r="D72" s="4">
-        <v>511.97637360948556</v>
+        <v>502.18679796742538</v>
       </c>
       <c r="E72" s="6">
         <v>11.333333333333321</v>
       </c>
       <c r="F72" s="6">
-        <v>0.79228691350726876</v>
+        <v>1.0095966128043301</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -1856,13 +1856,13 @@
         <v>2766.8669999999997</v>
       </c>
       <c r="D73" s="4">
-        <v>512.787626811677</v>
+        <v>503.19211796730451</v>
       </c>
       <c r="E73" s="6">
         <v>11.380952380952369</v>
       </c>
       <c r="F73" s="6">
-        <v>0.81125320219143759</v>
+        <v>1.0053199998791342</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -1876,13 +1876,13 @@
         <v>2785.7239999999997</v>
       </c>
       <c r="D74" s="4">
-        <v>513.61911001505632</v>
+        <v>504.19323186850602</v>
       </c>
       <c r="E74" s="6">
         <v>11.428571428571416</v>
       </c>
       <c r="F74" s="6">
-        <v>0.83148320337932091</v>
+        <v>1.0011139012015065</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -1896,13 +1896,13 @@
         <v>2804.5809999999997</v>
       </c>
       <c r="D75" s="4">
-        <v>514.47187447174929</v>
+        <v>505.19021902882616</v>
       </c>
       <c r="E75" s="6">
         <v>11.476190476190464</v>
       </c>
       <c r="F75" s="6">
-        <v>0.85276445669296663</v>
+        <v>0.99698716032014545</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -1916,13 +1916,13 @@
         <v>2823.4379999999996</v>
       </c>
       <c r="D76" s="4">
-        <v>515.34674803546204</v>
+        <v>506.18316737167925</v>
       </c>
       <c r="E76" s="6">
         <v>11.523809523809511</v>
       </c>
       <c r="F76" s="6">
-        <v>0.87487356371275382</v>
+        <v>0.99294834285308298</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -1936,13 +1936,13 @@
         <v>2842.2949999999996</v>
       </c>
       <c r="D77" s="4">
-        <v>516.24432552080816</v>
+        <v>507.17217310815965</v>
       </c>
       <c r="E77" s="6">
         <v>11.571428571428559</v>
       </c>
       <c r="F77" s="6">
-        <v>0.89757748534611892</v>
+        <v>0.9890057364804079</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -1956,13 +1956,13 @@
         <v>2861.1519999999996</v>
       </c>
       <c r="D78" s="4">
-        <v>517.16496044892392</v>
+        <v>508.15734045911472</v>
       </c>
       <c r="E78" s="6">
         <v>11.619047619047606</v>
       </c>
       <c r="F78" s="6">
-        <v>0.92063492811575998</v>
+        <v>0.98516735095506647</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -1976,13 +1976,13 @@
         <v>2880.0089999999996</v>
       </c>
       <c r="D79" s="4">
-        <v>518.1087582662467</v>
+        <v>509.13878137720485</v>
       </c>
       <c r="E79" s="6">
         <v>11.666666666666654</v>
       </c>
       <c r="F79" s="6">
-        <v>0.94379781732277479</v>
+        <v>0.98144091809012934</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -1996,13 +1996,13 @@
         <v>2898.8659999999995</v>
       </c>
       <c r="D80" s="4">
-        <v>519.0755711271222</v>
+        <v>510.1166152689774</v>
       </c>
       <c r="E80" s="6">
         <v>11.714285714285701</v>
       </c>
       <c r="F80" s="6">
-        <v>0.96681286087550689</v>
+        <v>0.97783389177254776</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -2016,13 +2016,13 @@
         <v>2917.7229999999995</v>
       </c>
       <c r="D81" s="4">
-        <v>520.0649943272756</v>
+        <v>511.09096871692896</v>
       </c>
       <c r="E81" s="6">
         <v>11.761904761904749</v>
       </c>
       <c r="F81" s="6">
-        <v>0.98942320015339646</v>
+        <v>0.97435344795155743</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -2036,13 +2036,13 @@
         <v>2936.58</v>
       </c>
       <c r="D82" s="4">
-        <v>521.07636447725508</v>
+        <v>512.06197520157366</v>
       </c>
       <c r="E82" s="6">
         <v>11.809523809523796</v>
       </c>
       <c r="F82" s="6">
-        <v>1.0113701499794843</v>
+        <v>0.97100648464470396</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -2056,13 +2056,13 @@
         <v>2955.4369999999999</v>
       </c>
       <c r="D83" s="4">
-        <v>522.10875950481113</v>
+        <v>513.02977482351025</v>
       </c>
       <c r="E83" s="6">
         <v>11.857142857142843</v>
       </c>
       <c r="F83" s="6">
-        <v>1.0323950275560492</v>
+        <v>0.9677996219365923</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -2076,13 +2076,13 @@
         <v>2974.2939999999999</v>
       </c>
       <c r="D84" s="4">
-        <v>523.16100057359563</v>
+        <v>513.9945140254888</v>
       </c>
       <c r="E84" s="6">
         <v>11.904761904761891</v>
       </c>
       <c r="F84" s="6">
-        <v>1.0522410687844967</v>
+        <v>0.96473920197854568</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -2096,13 +2096,13 @@
         <v>2993.1509999999998</v>
       </c>
       <c r="D85" s="4">
-        <v>524.23165600931225</v>
+        <v>514.95634531447763</v>
       </c>
       <c r="E85" s="6">
         <v>11.952380952380938</v>
       </c>
       <c r="F85" s="6">
-        <v>1.0706554357166169</v>
+        <v>0.96183128898883297</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2116,13 +2116,13 @@
         <v>3012.0079999999998</v>
       </c>
       <c r="D86" s="4">
-        <v>525.31904731693339</v>
+        <v>515.91542698373041</v>
       </c>
       <c r="E86" s="6">
         <v>12</v>
       </c>
       <c r="F86" s="6">
-        <v>1.0873913076211466</v>
+        <v>0.95908166925278238</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2136,13 +2136,13 @@
         <v>3030.8649999999998</v>
       </c>
       <c r="D87" s="4">
-        <v>526.42125738526647</v>
+        <v>516.87192283485228</v>
       </c>
       <c r="E87" s="6">
         <v>12</v>
       </c>
       <c r="F87" s="6">
-        <v>1.1022100683330791</v>
+        <v>0.95649585112187197</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -2156,13 +2156,13 @@
         <v>3049.7219999999998</v>
       </c>
       <c r="D88" s="4">
-        <v>527.53614095857029</v>
+        <v>517.82600189986965</v>
       </c>
       <c r="E88" s="6">
         <v>12</v>
       </c>
       <c r="F88" s="6">
-        <v>1.114883573303814</v>
+        <v>0.95407906501736761</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -2176,13 +2176,13 @@
         <v>3068.5789999999997</v>
       </c>
       <c r="D89" s="4">
-        <v>528.66133747119875</v>
+        <v>518.77783816329134</v>
       </c>
       <c r="E89" s="6">
         <v>12</v>
       </c>
       <c r="F89" s="6">
-        <v>1.1251965126284631</v>
+        <v>0.95183626342168282</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2196,13 +2196,13 @@
         <v>3087.4359999999997</v>
       </c>
       <c r="D90" s="4">
-        <v>529.79428632938198</v>
+        <v>519.72761028418267</v>
       </c>
       <c r="E90" s="6">
         <v>12</v>
       </c>
       <c r="F90" s="6">
-        <v>1.1329488581832265</v>
+        <v>0.949772120891339</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -2216,13 +2216,13 @@
         <v>3106.2929999999997</v>
       </c>
       <c r="D91" s="4">
-        <v>530.93224473091232</v>
+        <v>520.67550131822736</v>
       </c>
       <c r="E91" s="6">
         <v>12</v>
       </c>
       <c r="F91" s="6">
-        <v>1.1379584015303408</v>
+        <v>0.94789103404468733</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -2236,13 +2236,13 @@
         <v>3125.1499999999996</v>
       </c>
       <c r="D92" s="4">
-        <v>532.07230810979945</v>
+        <v>521.62169843979495</v>
       </c>
       <c r="E92" s="6">
         <v>12</v>
       </c>
       <c r="F92" s="6">
-        <v>1.1400633788871346</v>
+        <v>0.94619712156759306</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -2256,13 +2256,13 @@
         <v>3144.0069999999996</v>
       </c>
       <c r="D93" s="4">
-        <v>533.21143329629831</v>
+        <v>522.56639266401044</v>
       </c>
       <c r="E93" s="6">
         <v>12</v>
       </c>
       <c r="F93" s="6">
-        <v>1.139125186498859</v>
+        <v>0.94469422421548188</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2276,13 +2276,13 @@
         <v>3162.8639999999996</v>
       </c>
       <c r="D94" s="4">
-        <v>534.34646447895193</v>
+        <v>523.50977856881786</v>
       </c>
       <c r="E94" s="6">
         <v>12</v>
       </c>
       <c r="F94" s="6">
-        <v>1.1350311826536199</v>
+        <v>0.94338590480742823</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -2296,13 +2296,13 @@
         <v>3181.7209999999995</v>
       </c>
       <c r="D95" s="4">
-        <v>535.47416205867466</v>
+        <v>524.4520540170497</v>
       </c>
       <c r="E95" s="6">
         <v>12</v>
       </c>
       <c r="F95" s="6">
-        <v>1.1276975797227351</v>
+        <v>0.94227544823183962</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -2316,13 +2316,13 @@
         <v>3200.5779999999995</v>
       </c>
       <c r="D96" s="4">
-        <v>536.59123448258015</v>
+        <v>525.39341987849411</v>
       </c>
       <c r="E96" s="6">
         <v>12</v>
       </c>
       <c r="F96" s="6">
-        <v>1.1170724239054834</v>
+        <v>0.94136586144441026</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -2336,13 +2336,13 @@
         <v>3219.4349999999995</v>
       </c>
       <c r="D97" s="4">
-        <v>537.69437314648803</v>
+        <v>526.33407975195723</v>
       </c>
       <c r="E97" s="6">
         <v>12</v>
       </c>
       <c r="F97" s="6">
-        <v>1.1031386639078846</v>
+        <v>0.94065987346311886</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -2356,13 +2356,13 @@
         <v>3238.2919999999995</v>
       </c>
       <c r="D98" s="4">
-        <v>538.780290455451</v>
+        <v>527.27423968733729</v>
       </c>
       <c r="E98" s="6">
         <v>12</v>
       </c>
       <c r="F98" s="6">
-        <v>1.0859173089629621</v>
+        <v>0.94015993538005205</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -2376,13 +2376,13 @@
         <v>3257.1489999999999</v>
       </c>
       <c r="D99" s="4">
-        <v>539.8457611285221</v>
+        <v>528.2141079076855</v>
       </c>
       <c r="E99" s="6">
         <v>12</v>
       </c>
       <c r="F99" s="6">
-        <v>1.0654706730711041</v>
+        <v>0.93986822034821671</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -2396,13 +2396,13 @@
         <v>3276.0059999999999</v>
       </c>
       <c r="D100" s="4">
-        <v>540.88766683915583</v>
+        <v>529.15389453127659</v>
       </c>
       <c r="E100" s="6">
         <v>12</v>
       </c>
       <c r="F100" s="6">
-        <v>1.0419057106337277</v>
+        <v>0.93978662359108966</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -2416,13 +2416,13 @@
         <v>3294.8629999999998</v>
       </c>
       <c r="D101" s="4">
-        <v>541.90304427858337</v>
+        <v>530.0938112936733</v>
       </c>
       <c r="E101" s="6">
         <v>12</v>
       </c>
       <c r="F101" s="6">
-        <v>1.0153774394275388</v>
+        <v>0.93991676239670596</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -2436,13 +2436,13 @@
         <v>3313.72</v>
       </c>
       <c r="D102" s="4">
-        <v>542.8891367293063</v>
+        <v>531.03407126979482</v>
       </c>
       <c r="E102" s="6">
         <v>12</v>
       </c>
       <c r="F102" s="6">
-        <v>0.98609245072293561</v>
+        <v>0.94025997612152423</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -2456,13 +2456,13 @@
         <v>3332.5769999999998</v>
       </c>
       <c r="D103" s="4">
-        <v>543.84344924153538</v>
+        <v>531.97488859598343</v>
       </c>
       <c r="E103" s="6">
         <v>12</v>
       </c>
       <c r="F103" s="6">
-        <v>0.95431251222908031</v>
+        <v>0.94081732618860769</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -2476,13 +2476,13 @@
         <v>3351.4339999999997</v>
       </c>
       <c r="D104" s="4">
-        <v>544.76380749487271</v>
+        <v>532.91647819206969</v>
       </c>
       <c r="E104" s="6">
         <v>12</v>
       </c>
       <c r="F104" s="6">
-        <v>0.92035825333732646</v>
+        <v>0.94158959608625992</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -2496,13 +2496,13 @@
         <v>3370.2909999999997</v>
       </c>
       <c r="D105" s="4">
-        <v>545.64842043987574</v>
+        <v>533.8590554834459</v>
       </c>
       <c r="E105" s="6">
         <v>12</v>
       </c>
       <c r="F105" s="6">
-        <v>0.88461294500302756</v>
+        <v>0.94257729137621027</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -2516,13 +2516,13 @@
         <v>3389.1479999999997</v>
       </c>
       <c r="D106" s="4">
-        <v>546.49594680383143</v>
+        <v>534.80283612312223</v>
       </c>
       <c r="E106" s="6">
         <v>12</v>
       </c>
       <c r="F106" s="6">
-        <v>0.84752636395569425</v>
+        <v>0.94378063967633352</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -2536,13 +2536,13 @@
         <v>3408.0049999999997</v>
       </c>
       <c r="D107" s="4">
-        <v>547.30556555283238</v>
+        <v>535.74803571380176</v>
       </c>
       <c r="E107" s="6">
         <v>12</v>
       </c>
       <c r="F107" s="6">
-        <v>0.80961874900094699</v>
+        <v>0.94519959067952186</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -2556,13 +2556,13 @@
         <v>3426.8619999999996</v>
       </c>
       <c r="D108" s="4">
-        <v>548.07705039452685</v>
+        <v>536.6948695299468</v>
       </c>
       <c r="E108" s="6">
         <v>12</v>
       </c>
       <c r="F108" s="6">
-        <v>0.77148484169447329</v>
+        <v>0.94683381614504469</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -2576,13 +2576,13 @@
         <v>3445.7189999999996</v>
       </c>
       <c r="D109" s="4">
-        <v>548.81084841503161</v>
+        <v>537.6435522398433</v>
       </c>
       <c r="E109" s="6">
         <v>12</v>
       </c>
       <c r="F109" s="6">
-        <v>0.73379802050476428</v>
+        <v>0.94868270989650227</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -2596,13 +2596,13 @@
         <v>3464.5759999999996</v>
       </c>
       <c r="D110" s="4">
-        <v>549.50816293253138</v>
+        <v>538.5942976276649</v>
       </c>
       <c r="E110" s="6">
         <v>12</v>
       </c>
       <c r="F110" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.95074538782159834</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -2610,19 +2610,19 @@
         <v>181</v>
       </c>
       <c r="B111" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C111" s="4">
         <v>3483.4329999999995</v>
       </c>
       <c r="D111" s="4">
-        <v>595</v>
+        <v>539.54731831555114</v>
       </c>
       <c r="E111" s="6">
         <v>12</v>
       </c>
       <c r="F111" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.95302068788623728</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -2630,19 +2630,19 @@
         <v>182</v>
       </c>
       <c r="B112" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C112" s="4">
         <v>3502.2899999999995</v>
       </c>
       <c r="D112" s="4">
-        <v>595</v>
+        <v>540.50282548565883</v>
       </c>
       <c r="E112" s="6">
         <v>12</v>
       </c>
       <c r="F112" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.95550717010769404</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -2650,19 +2650,19 @@
         <v>183</v>
       </c>
       <c r="B113" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C113" s="4">
         <v>3521.1469999999995</v>
       </c>
       <c r="D113" s="4">
-        <v>595</v>
+        <v>541.46102860224323</v>
       </c>
       <c r="E113" s="6">
         <v>12</v>
       </c>
       <c r="F113" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.95820311658440005</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -2670,19 +2670,19 @@
         <v>184</v>
       </c>
       <c r="B114" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C114" s="4">
         <v>3540.0039999999999</v>
       </c>
       <c r="D114" s="4">
-        <v>595</v>
+        <v>542.42213513371667</v>
       </c>
       <c r="E114" s="6">
         <v>12</v>
       </c>
       <c r="F114" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.96110653147343328</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -2690,19 +2690,19 @@
         <v>185</v>
       </c>
       <c r="B115" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C115" s="4">
         <v>3558.8609999999999</v>
       </c>
       <c r="D115" s="4">
-        <v>595</v>
+        <v>543.38635027471355</v>
       </c>
       <c r="E115" s="6">
         <v>12</v>
       </c>
       <c r="F115" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.96421514099688466</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -2710,19 +2710,19 @@
         <v>186</v>
       </c>
       <c r="B116" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C116" s="4">
         <v>3577.7179999999998</v>
       </c>
       <c r="D116" s="4">
-        <v>595</v>
+        <v>544.35387666816905</v>
       </c>
       <c r="E116" s="6">
         <v>12</v>
       </c>
       <c r="F116" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.96752639345550051</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -2730,19 +2730,19 @@
         <v>187</v>
       </c>
       <c r="B117" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C117" s="4">
         <v>3596.5749999999998</v>
       </c>
       <c r="D117" s="4">
-        <v>595</v>
+        <v>545.32491412737158</v>
       </c>
       <c r="E117" s="6">
         <v>12</v>
       </c>
       <c r="F117" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.97103745920253459</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -2750,19 +2750,19 @@
         <v>188</v>
       </c>
       <c r="B118" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C118" s="4">
         <v>3615.4319999999998</v>
       </c>
       <c r="D118" s="4">
-        <v>595</v>
+        <v>546.29965935804012</v>
       </c>
       <c r="E118" s="6">
         <v>12</v>
       </c>
       <c r="F118" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.9747452306685318</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -2770,19 +2770,19 @@
         <v>189</v>
       </c>
       <c r="B119" s="3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C119" s="4">
         <v>3634.2889999999998</v>
       </c>
       <c r="D119" s="4">
-        <v>595</v>
+        <v>547.27830568038462</v>
       </c>
       <c r="E119" s="6">
         <v>12</v>
       </c>
       <c r="F119" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.97864632234450255</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -2790,19 +2790,19 @@
         <v>190</v>
       </c>
       <c r="B120" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C120" s="4">
         <v>3653.1459999999997</v>
       </c>
       <c r="D120" s="4">
-        <v>595</v>
+        <v>548.26104275117973</v>
       </c>
       <c r="E120" s="6">
         <v>12</v>
       </c>
       <c r="F120" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.98273707079511041</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -2810,19 +2810,19 @@
         <v>191</v>
       </c>
       <c r="B121" s="3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C121" s="4">
         <v>3672.0029999999997</v>
       </c>
       <c r="D121" s="4">
-        <v>595</v>
+        <v>549.24805628582385</v>
       </c>
       <c r="E121" s="6">
         <v>12</v>
       </c>
       <c r="F121" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.98701353464412023</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -2830,19 +2830,19 @@
         <v>192</v>
       </c>
       <c r="B122" s="3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C122" s="4">
         <v>3690.8599999999997</v>
       </c>
       <c r="D122" s="4">
-        <v>595</v>
+        <v>550.23952778041166</v>
       </c>
       <c r="E122" s="6">
         <v>12</v>
       </c>
       <c r="F122" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.99147149458781314</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -2850,19 +2850,19 @@
         <v>193</v>
       </c>
       <c r="B123" s="3">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C123" s="4">
         <v>3709.7169999999996</v>
       </c>
       <c r="D123" s="4">
-        <v>595</v>
+        <v>551.23563423379869</v>
       </c>
       <c r="E123" s="6">
         <v>12</v>
       </c>
       <c r="F123" s="6">
-        <v>0.69731451749976259</v>
+        <v>0.99610645338702852</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -2870,19 +2870,19 @@
         <v>194</v>
       </c>
       <c r="B124" s="3">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C124" s="4">
         <v>3728.5739999999996</v>
       </c>
       <c r="D124" s="4">
-        <v>595</v>
+        <v>552.23654786966949</v>
       </c>
       <c r="E124" s="6">
         <v>12</v>
       </c>
       <c r="F124" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.000913635870802</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -2890,19 +2890,19 @@
         <v>195</v>
       </c>
       <c r="B125" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C125" s="4">
         <v>3747.4309999999996</v>
       </c>
       <c r="D125" s="4">
-        <v>595</v>
+        <v>553.24243585860495</v>
       </c>
       <c r="E125" s="6">
         <v>12</v>
       </c>
       <c r="F125" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0058879889354557</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -2910,19 +2910,19 @@
         <v>196</v>
       </c>
       <c r="B126" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C126" s="4">
         <v>3766.2879999999996</v>
       </c>
       <c r="D126" s="4">
-        <v>595</v>
+        <v>554.25346004014455</v>
       </c>
       <c r="E126" s="6">
         <v>12</v>
       </c>
       <c r="F126" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0110241815395966</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -2930,19 +2930,19 @@
         <v>197</v>
       </c>
       <c r="B127" s="3">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C127" s="4">
         <v>3785.1449999999995</v>
       </c>
       <c r="D127" s="4">
-        <v>595</v>
+        <v>555.26977664486208</v>
       </c>
       <c r="E127" s="6">
         <v>12</v>
       </c>
       <c r="F127" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0163166047175309</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -2950,19 +2950,19 @@
         <v>198</v>
       </c>
       <c r="B128" s="3">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C128" s="4">
         <v>3804.0019999999995</v>
       </c>
       <c r="D128" s="4">
-        <v>595</v>
+        <v>556.29153601642247</v>
       </c>
       <c r="E128" s="6">
         <v>12</v>
       </c>
       <c r="F128" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0217593715603925</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -2970,19 +2970,19 @@
         <v>199</v>
       </c>
       <c r="B129" s="3">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C129" s="4">
         <v>3822.8589999999995</v>
       </c>
       <c r="D129" s="4">
-        <v>595</v>
+        <v>557.31888233365726</v>
       </c>
       <c r="E129" s="6">
         <v>12</v>
       </c>
       <c r="F129" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0273463172347874</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -2990,19 +2990,19 @@
         <v>200</v>
       </c>
       <c r="B130" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C130" s="4">
         <v>3841.7159999999994</v>
       </c>
       <c r="D130" s="4">
-        <v>595</v>
+        <v>558.35195333262686</v>
       </c>
       <c r="E130" s="6">
         <v>12</v>
       </c>
       <c r="F130" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0330709989696061</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -3010,19 +3010,19 @@
         <v>201</v>
       </c>
       <c r="B131" s="3">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C131" s="4">
         <v>3860.5729999999999</v>
       </c>
       <c r="D131" s="4">
-        <v>595</v>
+        <v>559.39088002868743</v>
       </c>
       <c r="E131" s="6">
         <v>12</v>
       </c>
       <c r="F131" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.038926696060571</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -3030,19 +3030,19 @@
         <v>202</v>
       </c>
       <c r="B132" s="3">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C132" s="4">
         <v>3879.43</v>
       </c>
       <c r="D132" s="4">
-        <v>595</v>
+        <v>560.43578643855926</v>
       </c>
       <c r="E132" s="6">
         <v>12</v>
       </c>
       <c r="F132" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0449064098718281</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
@@ -3050,19 +3050,19 @@
         <v>203</v>
       </c>
       <c r="B133" s="3">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C133" s="4">
         <v>3898.2869999999998</v>
       </c>
       <c r="D133" s="4">
-        <v>595</v>
+        <v>561.48678930239589</v>
       </c>
       <c r="E133" s="6">
         <v>12</v>
       </c>
       <c r="F133" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0510028638366293</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -3070,19 +3070,19 @@
         <v>204</v>
       </c>
       <c r="B134" s="3">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C134" s="4">
         <v>3917.1439999999998</v>
       </c>
       <c r="D134" s="4">
-        <v>595</v>
+        <v>562.54399780584458</v>
       </c>
       <c r="E134" s="6">
         <v>12</v>
       </c>
       <c r="F134" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0572085034486918</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -3090,19 +3090,19 @@
         <v>205</v>
       </c>
       <c r="B135" s="3">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C135" s="4">
         <v>3936.0009999999997</v>
       </c>
       <c r="D135" s="4">
-        <v>595</v>
+        <v>563.60751330212133</v>
       </c>
       <c r="E135" s="6">
         <v>12</v>
       </c>
       <c r="F135" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0635154962767501</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -3110,19 +3110,19 @@
         <v>206</v>
       </c>
       <c r="B136" s="3">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C136" s="4">
         <v>3954.8579999999997</v>
       </c>
       <c r="D136" s="4">
-        <v>595</v>
+        <v>564.67742903406975</v>
       </c>
       <c r="E136" s="6">
         <v>12</v>
       </c>
       <c r="F136" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0699157319484129</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
@@ -3130,19 +3130,19 @@
         <v>207</v>
       </c>
       <c r="B137" s="3">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="C137" s="4">
         <v>3973.7149999999997</v>
       </c>
       <c r="D137" s="4">
-        <v>595</v>
+        <v>565.75382985623469</v>
       </c>
       <c r="E137" s="6">
         <v>12</v>
       </c>
       <c r="F137" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0764008221649419</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -3150,19 +3150,19 @@
         <v>208</v>
       </c>
       <c r="B138" s="3">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C138" s="4">
         <v>3992.5719999999997</v>
       </c>
       <c r="D138" s="4">
-        <v>595</v>
+        <v>566.83679195692412</v>
       </c>
       <c r="E138" s="6">
         <v>12</v>
       </c>
       <c r="F138" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0829621006894286</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
@@ -3170,19 +3170,19 @@
         <v>209</v>
       </c>
       <c r="B139" s="3">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C139" s="4">
         <v>4011.4289999999996</v>
       </c>
       <c r="D139" s="4">
-        <v>595</v>
+        <v>567.92638258028092</v>
       </c>
       <c r="E139" s="6">
         <v>12</v>
       </c>
       <c r="F139" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0895906233567985</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -3190,19 +3190,19 @@
         <v>210</v>
       </c>
       <c r="B140" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C140" s="4">
         <v>4030.2859999999996</v>
       </c>
       <c r="D140" s="4">
-        <v>595</v>
+        <v>569.02265974834449</v>
       </c>
       <c r="E140" s="6">
         <v>12</v>
       </c>
       <c r="F140" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.0962771680635797</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -3210,19 +3210,19 @@
         <v>211</v>
       </c>
       <c r="B141" s="3">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C141" s="4">
         <v>4049.1429999999996</v>
       </c>
       <c r="D141" s="4">
-        <v>595</v>
+        <v>570.12567198312217</v>
       </c>
       <c r="E141" s="6">
         <v>12</v>
       </c>
       <c r="F141" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1030122347776796</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -3230,19 +3230,19 @@
         <v>212</v>
       </c>
       <c r="B142" s="3">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C142" s="4">
         <v>4067.9999999999995</v>
       </c>
       <c r="D142" s="4">
-        <v>595</v>
+        <v>571.2354580286551</v>
       </c>
       <c r="E142" s="6">
         <v>12</v>
       </c>
       <c r="F142" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1097860455329283</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
@@ -3250,19 +3250,19 @@
         <v>213</v>
       </c>
       <c r="B143" s="3">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C143" s="4">
         <v>4086.8569999999995</v>
       </c>
       <c r="D143" s="4">
-        <v>595</v>
+        <v>572.352046573081</v>
       </c>
       <c r="E143" s="6">
         <v>12</v>
       </c>
       <c r="F143" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1165885444258947</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -3270,19 +3270,19 @@
         <v>214</v>
       </c>
       <c r="B144" s="3">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="C144" s="4">
         <v>4105.7139999999999</v>
       </c>
       <c r="D144" s="4">
-        <v>595</v>
+        <v>573.47545597070825</v>
       </c>
       <c r="E144" s="6">
         <v>12</v>
       </c>
       <c r="F144" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1234093976272561</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
@@ -3290,19 +3290,19 @@
         <v>215</v>
       </c>
       <c r="B145" s="3">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C145" s="4">
         <v>4124.5709999999999</v>
       </c>
       <c r="D145" s="4">
-        <v>595</v>
+        <v>574.60569396407573</v>
       </c>
       <c r="E145" s="6">
         <v>12</v>
       </c>
       <c r="F145" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1302379933674729</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -3310,19 +3310,19 @@
         <v>216</v>
       </c>
       <c r="B146" s="3">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C146" s="4">
         <v>4143.4279999999999</v>
       </c>
       <c r="D146" s="4">
-        <v>595</v>
+        <v>575.74275740602639</v>
       </c>
       <c r="E146" s="6">
         <v>12</v>
       </c>
       <c r="F146" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1370634419506587</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
@@ -3330,19 +3330,19 @@
         <v>217</v>
       </c>
       <c r="B147" s="3">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="C147" s="4">
         <v>4162.2849999999999</v>
       </c>
       <c r="D147" s="4">
-        <v>595</v>
+        <v>576.88663198176869</v>
       </c>
       <c r="E147" s="6">
         <v>12</v>
       </c>
       <c r="F147" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1438745757423021</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
@@ -3350,19 +3350,19 @@
         <v>218</v>
       </c>
       <c r="B148" s="3">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="C148" s="4">
         <v>4181.1419999999998</v>
       </c>
       <c r="D148" s="4">
-        <v>595</v>
+        <v>578.03729193094568</v>
       </c>
       <c r="E148" s="6">
         <v>12</v>
       </c>
       <c r="F148" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1506599491769975</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
@@ -3370,19 +3370,19 @@
         <v>219</v>
       </c>
       <c r="B149" s="3">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="C149" s="4">
         <v>4199.9989999999998</v>
       </c>
       <c r="D149" s="4">
-        <v>595</v>
+        <v>579.19469976970504</v>
       </c>
       <c r="E149" s="6">
         <v>12</v>
       </c>
       <c r="F149" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1574078387593545</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
@@ -3390,19 +3390,19 @@
         <v>220</v>
       </c>
       <c r="B150" s="3">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C150" s="4">
         <v>4218.8559999999998</v>
       </c>
       <c r="D150" s="4">
-        <v>595</v>
+        <v>580.35880601275699</v>
       </c>
       <c r="E150" s="6">
         <v>12</v>
       </c>
       <c r="F150" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1641062430519469</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
@@ -3410,19 +3410,19 @@
         <v>221</v>
       </c>
       <c r="B151" s="3">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="C151" s="4">
         <v>4237.7129999999997</v>
       </c>
       <c r="D151" s="4">
-        <v>595</v>
+        <v>581.52954889545254</v>
       </c>
       <c r="E151" s="6">
         <v>12</v>
       </c>
       <c r="F151" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1707428826955493</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -3430,19 +3430,19 @@
         <v>222</v>
       </c>
       <c r="B152" s="3">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="C152" s="4">
         <v>4256.57</v>
       </c>
       <c r="D152" s="4">
-        <v>595</v>
+        <v>582.70685409584348</v>
       </c>
       <c r="E152" s="6">
         <v>12</v>
       </c>
       <c r="F152" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.177305200390947</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
@@ -3450,19 +3450,19 @@
         <v>223</v>
       </c>
       <c r="B153" s="3">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="C153" s="4">
         <v>4275.4269999999997</v>
       </c>
       <c r="D153" s="4">
-        <v>595</v>
+        <v>583.89063445674924</v>
       </c>
       <c r="E153" s="6">
         <v>12</v>
       </c>
       <c r="F153" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1837803609057573</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
@@ -3470,19 +3470,19 @@
         <v>224</v>
       </c>
       <c r="B154" s="3">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="C154" s="4">
         <v>4294.2839999999997</v>
       </c>
       <c r="D154" s="4">
-        <v>595</v>
+        <v>585.08078970782867</v>
       </c>
       <c r="E154" s="6">
         <v>12</v>
       </c>
       <c r="F154" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1901552510794318</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
@@ -3490,19 +3490,19 @@
         <v>225</v>
       </c>
       <c r="B155" s="3">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C155" s="4">
         <v>4313.1409999999996</v>
       </c>
       <c r="D155" s="4">
-        <v>595</v>
+        <v>586.27720618763942</v>
       </c>
       <c r="E155" s="6">
         <v>12</v>
       </c>
       <c r="F155" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.1964164798107504</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -3510,19 +3510,19 @@
         <v>226</v>
       </c>
       <c r="B156" s="3">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="C156" s="4">
         <v>4331.9979999999996</v>
       </c>
       <c r="D156" s="4">
-        <v>595</v>
+        <v>587.47975656571202</v>
       </c>
       <c r="E156" s="6">
         <v>12</v>
       </c>
       <c r="F156" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2025503780726012</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -3530,19 +3530,19 @@
         <v>227</v>
       </c>
       <c r="B157" s="3">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="C157" s="4">
         <v>4350.8549999999996</v>
       </c>
       <c r="D157" s="4">
-        <v>595</v>
+        <v>588.68829956461445</v>
       </c>
       <c r="E157" s="6">
         <v>12</v>
       </c>
       <c r="F157" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2085429989024306</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
@@ -3550,19 +3550,19 @@
         <v>228</v>
       </c>
       <c r="B158" s="3">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="C158" s="4">
         <v>4369.7119999999995</v>
       </c>
       <c r="D158" s="4">
-        <v>595</v>
+        <v>589.90267968201533</v>
       </c>
       <c r="E158" s="6">
         <v>12</v>
       </c>
       <c r="F158" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2143801174008786</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
@@ -3570,19 +3570,19 @@
         <v>229</v>
       </c>
       <c r="B159" s="3">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="C159" s="4">
         <v>4388.5689999999995</v>
       </c>
       <c r="D159" s="4">
-        <v>595</v>
+        <v>591.12272691275916</v>
       </c>
       <c r="E159" s="6">
         <v>12</v>
       </c>
       <c r="F159" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2200472307438304</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
@@ -3590,19 +3590,19 @@
         <v>230</v>
       </c>
       <c r="B160" s="3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C160" s="4">
         <v>4407.4259999999995</v>
       </c>
       <c r="D160" s="4">
-        <v>595</v>
+        <v>592.34825647092271</v>
       </c>
       <c r="E160" s="6">
         <v>12</v>
       </c>
       <c r="F160" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2255295581635437</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
@@ -3610,19 +3610,19 @@
         <v>231</v>
       </c>
       <c r="B161" s="3">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="C161" s="4">
         <v>4426.2829999999994</v>
       </c>
       <c r="D161" s="4">
-        <v>595</v>
+        <v>593.57906851188955</v>
       </c>
       <c r="E161" s="6">
         <v>12</v>
       </c>
       <c r="F161" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.230812040966839</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
@@ -3630,19 +3630,19 @@
         <v>232</v>
       </c>
       <c r="B162" s="3">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="C162" s="4">
         <v>4445.1399999999994</v>
       </c>
       <c r="D162" s="4">
-        <v>595</v>
+        <v>594.81494785441873</v>
       </c>
       <c r="E162" s="6">
         <v>12</v>
       </c>
       <c r="F162" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2358793425291879</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
@@ -3650,19 +3650,19 @@
         <v>233</v>
       </c>
       <c r="B163" s="3">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="C163" s="4">
         <v>4463.9969999999994</v>
       </c>
       <c r="D163" s="4">
-        <v>595</v>
+        <v>596.05566370270139</v>
       </c>
       <c r="E163" s="6">
         <v>12</v>
       </c>
       <c r="F163" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2407158482826617</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
@@ -3670,19 +3670,19 @@
         <v>234</v>
       </c>
       <c r="B164" s="3">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="C164" s="4">
         <v>4482.8539999999994</v>
       </c>
       <c r="D164" s="4">
-        <v>595</v>
+        <v>597.3009693684362</v>
       </c>
       <c r="E164" s="6">
         <v>12</v>
       </c>
       <c r="F164" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2453056657348043</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
@@ -3690,19 +3690,19 @@
         <v>235</v>
       </c>
       <c r="B165" s="3">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="C165" s="4">
         <v>4501.7109999999993</v>
       </c>
       <c r="D165" s="4">
-        <v>595</v>
+        <v>598.5506019928971</v>
       </c>
       <c r="E165" s="6">
         <v>12</v>
       </c>
       <c r="F165" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2496326244609008</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
@@ -3710,19 +3710,19 @@
         <v>236</v>
       </c>
       <c r="B166" s="3">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="C166" s="4">
         <v>4520.5679999999993</v>
       </c>
       <c r="D166" s="4">
-        <v>595</v>
+        <v>599.80428226899562</v>
       </c>
       <c r="E166" s="6">
         <v>12</v>
       </c>
       <c r="F166" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2536802760985211</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
@@ -3730,19 +3730,19 @@
         <v>237</v>
       </c>
       <c r="B167" s="3">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="C167" s="4">
         <v>4539.4249999999993</v>
       </c>
       <c r="D167" s="4">
-        <v>595</v>
+        <v>601.06171416334632</v>
       </c>
       <c r="E167" s="6">
         <v>12</v>
       </c>
       <c r="F167" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2574318943507024</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
@@ -3750,19 +3750,19 @@
         <v>238</v>
       </c>
       <c r="B168" s="3">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="C168" s="4">
         <v>4558.2819999999992</v>
       </c>
       <c r="D168" s="4">
-        <v>595</v>
+        <v>602.32258463834251</v>
       </c>
       <c r="E168" s="6">
         <v>12</v>
       </c>
       <c r="F168" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2608704749961817</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
@@ -3770,19 +3770,19 @@
         <v>239</v>
       </c>
       <c r="B169" s="3">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="C169" s="4">
         <v>4577.1389999999992</v>
       </c>
       <c r="D169" s="4">
-        <v>595</v>
+        <v>603.58656337421075</v>
       </c>
       <c r="E169" s="6">
         <v>12</v>
       </c>
       <c r="F169" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2639787358682497</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
@@ -3790,19 +3790,19 @@
         <v>240</v>
       </c>
       <c r="B170" s="3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C170" s="4">
         <v>4595.9960000000001</v>
       </c>
       <c r="D170" s="4">
-        <v>595</v>
+        <v>604.85330249109143</v>
       </c>
       <c r="E170" s="6">
         <v>12</v>
       </c>
       <c r="F170" s="6">
-        <v>0.69731451749976259</v>
+        <v>1.2667391168806716</v>
       </c>
     </row>
   </sheetData>

</xml_diff>